<commit_message>
fixed max case error
</commit_message>
<xml_diff>
--- a/outcome/appendix/Figure Data/Fig.4 data.xlsx
+++ b/outcome/appendix/Figure Data/Fig.4 data.xlsx
@@ -15039,19 +15039,19 @@
         <v>43831</v>
       </c>
       <c r="B2" t="n">
-        <v>2554.10102226337</v>
+        <v>2555.22214850378</v>
       </c>
       <c r="C2" t="n">
-        <v>1739.17348020312</v>
+        <v>1743.37403972035</v>
       </c>
       <c r="D2" t="n">
-        <v>1276.85835248462</v>
+        <v>1280.88312680667</v>
       </c>
       <c r="E2" t="n">
         <v>3271.60836224899</v>
       </c>
       <c r="F2" t="n">
-        <v>3676.33165698684</v>
+        <v>3681.26877844585</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -15060,7 +15060,7 @@
         <v>2445</v>
       </c>
       <c r="I2" t="n">
-        <v>109.101022263374</v>
+        <v>110.222148503781</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
@@ -15071,13 +15071,13 @@
         <v>43862</v>
       </c>
       <c r="B3" t="n">
-        <v>2597.23487376181</v>
+        <v>2597.49638362041</v>
       </c>
       <c r="C3" t="n">
-        <v>1559.52085799588</v>
+        <v>1560.58769315346</v>
       </c>
       <c r="D3" t="n">
-        <v>1183.64951344664</v>
+        <v>1186.10121510877</v>
       </c>
       <c r="E3" t="n">
         <v>3476.76635922184</v>
@@ -15092,7 +15092,7 @@
         <v>933</v>
       </c>
       <c r="I3" t="n">
-        <v>1664.23487376181</v>
+        <v>1664.49638362041</v>
       </c>
       <c r="J3" t="s">
         <v>11</v>
@@ -15103,13 +15103,13 @@
         <v>43891</v>
       </c>
       <c r="B4" t="n">
-        <v>4416.60559291829</v>
+        <v>4414.9056151499</v>
       </c>
       <c r="C4" t="n">
-        <v>3165.03960694311</v>
+        <v>3157.81603849888</v>
       </c>
       <c r="D4" t="n">
-        <v>2816.04143320464</v>
+        <v>2808.94044563282</v>
       </c>
       <c r="E4" t="n">
         <v>5596.16176007132</v>
@@ -15124,7 +15124,7 @@
         <v>3508</v>
       </c>
       <c r="I4" t="n">
-        <v>908.605592918292</v>
+        <v>906.905615149898</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
@@ -15135,7 +15135,7 @@
         <v>43922</v>
       </c>
       <c r="B5" t="n">
-        <v>4989.05769394917</v>
+        <v>4990.37131566918</v>
       </c>
       <c r="C5" t="n">
         <v>3698.61255729682</v>
@@ -15156,7 +15156,7 @@
         <v>5360</v>
       </c>
       <c r="I5" t="n">
-        <v>-370.942306050834</v>
+        <v>-369.628684330823</v>
       </c>
       <c r="J5" t="s">
         <v>12</v>
@@ -15167,13 +15167,13 @@
         <v>43952</v>
       </c>
       <c r="B6" t="n">
-        <v>5744.65007810336</v>
+        <v>5741.59408251857</v>
       </c>
       <c r="C6" t="n">
-        <v>4301.21663657899</v>
+        <v>4286.73455584564</v>
       </c>
       <c r="D6" t="n">
-        <v>3851.34267036954</v>
+        <v>3842.87151006306</v>
       </c>
       <c r="E6" t="n">
         <v>7364.26587048967</v>
@@ -15188,7 +15188,7 @@
         <v>5264</v>
       </c>
       <c r="I6" t="n">
-        <v>480.650078103359</v>
+        <v>477.594082518573</v>
       </c>
       <c r="J6" t="s">
         <v>11</v>
@@ -15199,10 +15199,10 @@
         <v>43983</v>
       </c>
       <c r="B7" t="n">
-        <v>5987.98297822111</v>
+        <v>5984.95544467332</v>
       </c>
       <c r="C7" t="n">
-        <v>4580.58024703117</v>
+        <v>4576.30137597937</v>
       </c>
       <c r="D7" t="n">
         <v>4024.01929999012</v>
@@ -15220,7 +15220,7 @@
         <v>6193</v>
       </c>
       <c r="I7" t="n">
-        <v>-205.017021778895</v>
+        <v>-208.04455532668</v>
       </c>
       <c r="J7" t="s">
         <v>12</v>
@@ -15231,7 +15231,7 @@
         <v>44013</v>
       </c>
       <c r="B8" t="n">
-        <v>5911.38237902578</v>
+        <v>5910.68186337853</v>
       </c>
       <c r="C8" t="n">
         <v>4508.01441521917</v>
@@ -15252,7 +15252,7 @@
         <v>4972</v>
       </c>
       <c r="I8" t="n">
-        <v>939.382379025783</v>
+        <v>938.68186337853</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
@@ -15263,7 +15263,7 @@
         <v>44044</v>
       </c>
       <c r="B9" t="n">
-        <v>5136.39445964404</v>
+        <v>5129.43375580138</v>
       </c>
       <c r="C9" t="n">
         <v>3704.75311686093</v>
@@ -15284,7 +15284,7 @@
         <v>4972</v>
       </c>
       <c r="I9" t="n">
-        <v>164.394459644041</v>
+        <v>157.433755801384</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
@@ -15295,7 +15295,7 @@
         <v>44075</v>
       </c>
       <c r="B10" t="n">
-        <v>3700.00165516157</v>
+        <v>3706.12156607305</v>
       </c>
       <c r="C10" t="n">
         <v>2280.91237764028</v>
@@ -15304,7 +15304,7 @@
         <v>1563.77012561258</v>
       </c>
       <c r="E10" t="n">
-        <v>5000.04276709215</v>
+        <v>5008.12892526094</v>
       </c>
       <c r="F10" t="n">
         <v>5707.48255306939</v>
@@ -15316,7 +15316,7 @@
         <v>4492</v>
       </c>
       <c r="I10" t="n">
-        <v>-791.998344838434</v>
+        <v>-785.878433926947</v>
       </c>
       <c r="J10" t="s">
         <v>12</v>
@@ -15327,7 +15327,7 @@
         <v>44105</v>
       </c>
       <c r="B11" t="n">
-        <v>2742.56824079948</v>
+        <v>2748.77064436662</v>
       </c>
       <c r="C11" t="n">
         <v>1270.95727147084</v>
@@ -15348,7 +15348,7 @@
         <v>3206</v>
       </c>
       <c r="I11" t="n">
-        <v>-463.431759200518</v>
+        <v>-457.229355633384</v>
       </c>
       <c r="J11" t="s">
         <v>12</v>
@@ -15359,7 +15359,7 @@
         <v>44136</v>
       </c>
       <c r="B12" t="n">
-        <v>2979.36432878185</v>
+        <v>2983.12915677683</v>
       </c>
       <c r="C12" t="n">
         <v>1485.16038457302</v>
@@ -15380,7 +15380,7 @@
         <v>3611</v>
       </c>
       <c r="I12" t="n">
-        <v>-631.635671218145</v>
+        <v>-627.870843223168</v>
       </c>
       <c r="J12" t="s">
         <v>12</v>
@@ -15391,7 +15391,7 @@
         <v>44166</v>
       </c>
       <c r="B13" t="n">
-        <v>3091.35024411299</v>
+        <v>3093.39154033956</v>
       </c>
       <c r="C13" t="n">
         <v>1495.37848461347</v>
@@ -15412,7 +15412,7 @@
         <v>3694</v>
       </c>
       <c r="I13" t="n">
-        <v>-602.649755887014</v>
+        <v>-600.608459660443</v>
       </c>
       <c r="J13" t="s">
         <v>12</v>
@@ -15423,7 +15423,7 @@
         <v>44197</v>
       </c>
       <c r="B14" t="n">
-        <v>2622.88347339437</v>
+        <v>2625.70802482369</v>
       </c>
       <c r="C14" t="n">
         <v>914.535566587633</v>
@@ -15444,7 +15444,7 @@
         <v>3175</v>
       </c>
       <c r="I14" t="n">
-        <v>-552.116526605628</v>
+        <v>-549.291975176315</v>
       </c>
       <c r="J14" t="s">
         <v>12</v>
@@ -15455,7 +15455,7 @@
         <v>44228</v>
       </c>
       <c r="B15" t="n">
-        <v>2632.46465252311</v>
+        <v>2633.47312104534</v>
       </c>
       <c r="C15" t="n">
         <v>1109.73360437002</v>
@@ -15476,7 +15476,7 @@
         <v>3425</v>
       </c>
       <c r="I15" t="n">
-        <v>-792.535347476892</v>
+        <v>-791.526878954662</v>
       </c>
       <c r="J15" t="s">
         <v>12</v>
@@ -15487,10 +15487,10 @@
         <v>44256</v>
       </c>
       <c r="B16" t="n">
-        <v>4437.39497955556</v>
+        <v>4433.73411459297</v>
       </c>
       <c r="C16" t="n">
-        <v>2886.60339072815</v>
+        <v>2863.079709259</v>
       </c>
       <c r="D16" t="n">
         <v>2104.9209996519</v>
@@ -15508,7 +15508,7 @@
         <v>7220</v>
       </c>
       <c r="I16" t="n">
-        <v>-2782.60502044444</v>
+        <v>-2786.26588540703</v>
       </c>
       <c r="J16" t="s">
         <v>12</v>
@@ -15519,7 +15519,7 @@
         <v>44287</v>
       </c>
       <c r="B17" t="n">
-        <v>5025.12820290517</v>
+        <v>5026.99262560956</v>
       </c>
       <c r="C17" t="n">
         <v>3212.30103585908</v>
@@ -15540,7 +15540,7 @@
         <v>7848</v>
       </c>
       <c r="I17" t="n">
-        <v>-2822.87179709483</v>
+        <v>-2821.00737439044</v>
       </c>
       <c r="J17" t="s">
         <v>12</v>
@@ -15551,7 +15551,7 @@
         <v>44317</v>
       </c>
       <c r="B18" t="n">
-        <v>5785.08781019604</v>
+        <v>5779.42662112342</v>
       </c>
       <c r="C18" t="n">
         <v>3974.86523006948</v>
@@ -15572,7 +15572,7 @@
         <v>8096</v>
       </c>
       <c r="I18" t="n">
-        <v>-2310.91218980396</v>
+        <v>-2316.57337887658</v>
       </c>
       <c r="J18" t="s">
         <v>12</v>
@@ -15583,7 +15583,7 @@
         <v>44348</v>
       </c>
       <c r="B19" t="n">
-        <v>6010.797131454</v>
+        <v>6004.73152874422</v>
       </c>
       <c r="C19" t="n">
         <v>4058.55539256903</v>
@@ -15604,7 +15604,7 @@
         <v>9670</v>
       </c>
       <c r="I19" t="n">
-        <v>-3659.202868546</v>
+        <v>-3665.26847125578</v>
       </c>
       <c r="J19" t="s">
         <v>12</v>
@@ -15615,7 +15615,7 @@
         <v>44378</v>
       </c>
       <c r="B20" t="n">
-        <v>5944.54721202949</v>
+        <v>5941.08861073059</v>
       </c>
       <c r="C20" t="n">
         <v>4015.74336863362</v>
@@ -15636,7 +15636,7 @@
         <v>9222</v>
       </c>
       <c r="I20" t="n">
-        <v>-3277.45278797051</v>
+        <v>-3280.91138926941</v>
       </c>
       <c r="J20" t="s">
         <v>12</v>
@@ -15647,7 +15647,7 @@
         <v>44409</v>
       </c>
       <c r="B21" t="n">
-        <v>5253.33452449487</v>
+        <v>5245.69238773845</v>
       </c>
       <c r="C21" t="n">
         <v>3168.01097141081</v>
@@ -15668,7 +15668,7 @@
         <v>6867</v>
       </c>
       <c r="I21" t="n">
-        <v>-1613.66547550513</v>
+        <v>-1621.30761226155</v>
       </c>
       <c r="J21" t="s">
         <v>12</v>
@@ -15679,7 +15679,7 @@
         <v>44440</v>
       </c>
       <c r="B22" t="n">
-        <v>3920.85801135977</v>
+        <v>3915.02352487536</v>
       </c>
       <c r="C22" t="n">
         <v>1596.28075551273</v>
@@ -15688,7 +15688,7 @@
         <v>516.716414998119</v>
       </c>
       <c r="E22" t="n">
-        <v>6026.76501089352</v>
+        <v>6018.59935900045</v>
       </c>
       <c r="F22" t="n">
         <v>6754.53626368385</v>
@@ -15700,7 +15700,7 @@
         <v>5932</v>
       </c>
       <c r="I22" t="n">
-        <v>-2011.14198864023</v>
+        <v>-2016.97647512464</v>
       </c>
       <c r="J22" t="s">
         <v>12</v>
@@ -15711,7 +15711,7 @@
         <v>44470</v>
       </c>
       <c r="B23" t="n">
-        <v>2898.0504144503</v>
+        <v>2908.29699784213</v>
       </c>
       <c r="C23" t="n">
         <v>609.066428788389</v>
@@ -15732,7 +15732,7 @@
         <v>3622</v>
       </c>
       <c r="I23" t="n">
-        <v>-723.9495855497</v>
+        <v>-713.703002157868</v>
       </c>
       <c r="J23" t="s">
         <v>12</v>
@@ -15743,7 +15743,7 @@
         <v>44501</v>
       </c>
       <c r="B24" t="n">
-        <v>3046.30590993045</v>
+        <v>3055.34389284321</v>
       </c>
       <c r="C24" t="n">
         <v>843.790364101251</v>
@@ -15764,7 +15764,7 @@
         <v>3649</v>
       </c>
       <c r="I24" t="n">
-        <v>-602.69409006955</v>
+        <v>-593.656107156793</v>
       </c>
       <c r="J24" t="s">
         <v>12</v>
@@ -15775,7 +15775,7 @@
         <v>44531</v>
       </c>
       <c r="B25" t="n">
-        <v>3144.89526588405</v>
+        <v>3149.30937091482</v>
       </c>
       <c r="C25" t="n">
         <v>872.665392514946</v>
@@ -15796,7 +15796,7 @@
         <v>4919</v>
       </c>
       <c r="I25" t="n">
-        <v>-1774.10473411595</v>
+        <v>-1769.69062908518</v>
       </c>
       <c r="J25" t="s">
         <v>12</v>
@@ -15807,7 +15807,7 @@
         <v>44562</v>
       </c>
       <c r="B26" t="n">
-        <v>2691.63169428851</v>
+        <v>2696.65476749499</v>
       </c>
       <c r="C26" t="n">
         <v>308.882650776172</v>
@@ -15828,7 +15828,7 @@
         <v>4396</v>
       </c>
       <c r="I26" t="n">
-        <v>-1704.36830571149</v>
+        <v>-1699.34523250501</v>
       </c>
       <c r="J26" t="s">
         <v>12</v>
@@ -15839,7 +15839,7 @@
         <v>44593</v>
       </c>
       <c r="B27" t="n">
-        <v>2707.16632124769</v>
+        <v>2709.30991602845</v>
       </c>
       <c r="C27" t="n">
         <v>519.769590278987</v>
@@ -15860,7 +15860,7 @@
         <v>4689</v>
       </c>
       <c r="I27" t="n">
-        <v>-1981.83367875231</v>
+        <v>-1979.69008397155</v>
       </c>
       <c r="J27" t="s">
         <v>12</v>
@@ -15871,7 +15871,7 @@
         <v>44621</v>
       </c>
       <c r="B28" t="n">
-        <v>4482.422913852</v>
+        <v>4476.71349127572</v>
       </c>
       <c r="C28" t="n">
         <v>2379.12502099825</v>
@@ -15892,7 +15892,7 @@
         <v>6656</v>
       </c>
       <c r="I28" t="n">
-        <v>-2173.577086148</v>
+        <v>-2179.28650872428</v>
       </c>
       <c r="J28" t="s">
         <v>12</v>
@@ -15903,7 +15903,7 @@
         <v>44652</v>
       </c>
       <c r="B29" t="n">
-        <v>5080.71316167371</v>
+        <v>5082.42689782692</v>
       </c>
       <c r="C29" t="n">
         <v>2684.47444578355</v>
@@ -15924,7 +15924,7 @@
         <v>7124</v>
       </c>
       <c r="I29" t="n">
-        <v>-2043.28683832629</v>
+        <v>-2041.57310217308</v>
       </c>
       <c r="J29" t="s">
         <v>12</v>
@@ -15935,7 +15935,7 @@
         <v>44682</v>
       </c>
       <c r="B30" t="n">
-        <v>5823.22673982214</v>
+        <v>5815.52486278837</v>
       </c>
       <c r="C30" t="n">
         <v>3384.15643212497</v>
@@ -15956,7 +15956,7 @@
         <v>8824</v>
       </c>
       <c r="I30" t="n">
-        <v>-3000.77326017786</v>
+        <v>-3008.47513721163</v>
       </c>
       <c r="J30" t="s">
         <v>12</v>
@@ -15967,7 +15967,7 @@
         <v>44713</v>
       </c>
       <c r="B31" t="n">
-        <v>6061.87246411206</v>
+        <v>6053.00337511718</v>
       </c>
       <c r="C31" t="n">
         <v>3505.68264104479</v>
@@ -15988,7 +15988,7 @@
         <v>9943</v>
       </c>
       <c r="I31" t="n">
-        <v>-3881.12753588794</v>
+        <v>-3889.99662488282</v>
       </c>
       <c r="J31" t="s">
         <v>12</v>
@@ -15999,7 +15999,7 @@
         <v>44743</v>
       </c>
       <c r="B32" t="n">
-        <v>6011.01386808144</v>
+        <v>6004.60073919966</v>
       </c>
       <c r="C32" t="n">
         <v>3509.73564091691</v>
@@ -16020,7 +16020,7 @@
         <v>9683</v>
       </c>
       <c r="I32" t="n">
-        <v>-3671.98613191856</v>
+        <v>-3678.39926080034</v>
       </c>
       <c r="J32" t="s">
         <v>12</v>
@@ -16031,7 +16031,7 @@
         <v>44774</v>
       </c>
       <c r="B33" t="n">
-        <v>5340.21922025988</v>
+        <v>5333.70617534132</v>
       </c>
       <c r="C33" t="n">
         <v>2604.02843513953</v>
@@ -16052,7 +16052,7 @@
         <v>7887</v>
       </c>
       <c r="I33" t="n">
-        <v>-2546.78077974012</v>
+        <v>-2553.29382465868</v>
       </c>
       <c r="J33" t="s">
         <v>12</v>
@@ -16063,7 +16063,7 @@
         <v>44805</v>
       </c>
       <c r="B34" t="n">
-        <v>4148.22252351995</v>
+        <v>4134.45614157218</v>
       </c>
       <c r="C34" t="n">
         <v>1089.52914902542</v>
@@ -16084,7 +16084,7 @@
         <v>5311</v>
       </c>
       <c r="I34" t="n">
-        <v>-1162.77747648005</v>
+        <v>-1176.54385842782</v>
       </c>
       <c r="J34" t="s">
         <v>12</v>
@@ -16095,7 +16095,7 @@
         <v>44835</v>
       </c>
       <c r="B35" t="n">
-        <v>3114.51763734401</v>
+        <v>3127.89732682456</v>
       </c>
       <c r="C35" t="n">
         <v>111.503518432598</v>
@@ -16116,7 +16116,7 @@
         <v>2535</v>
       </c>
       <c r="I35" t="n">
-        <v>579.51763734401</v>
+        <v>592.897326824562</v>
       </c>
       <c r="J35" t="s">
         <v>11</v>
@@ -16127,7 +16127,7 @@
         <v>44866</v>
       </c>
       <c r="B36" t="n">
-        <v>3135.74258148268</v>
+        <v>3152.63983680369</v>
       </c>
       <c r="C36" t="n">
         <v>354.926773711633</v>
@@ -16148,7 +16148,7 @@
         <v>2569</v>
       </c>
       <c r="I36" t="n">
-        <v>566.742581482679</v>
+        <v>583.639836803686</v>
       </c>
       <c r="J36" t="s">
         <v>11</v>
@@ -16159,7 +16159,7 @@
         <v>44896</v>
       </c>
       <c r="B37" t="n">
-        <v>3212.22309621244</v>
+        <v>3220.4066011882</v>
       </c>
       <c r="C37" t="n">
         <v>392.056211914838</v>
@@ -16180,7 +16180,7 @@
         <v>1820</v>
       </c>
       <c r="I37" t="n">
-        <v>1392.22309621244</v>
+        <v>1400.4066011882</v>
       </c>
       <c r="J37" t="s">
         <v>11</v>
@@ -16191,7 +16191,7 @@
         <v>44927</v>
       </c>
       <c r="B38" t="n">
-        <v>2759.92199785789</v>
+        <v>2767.72837158677</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -16212,7 +16212,7 @@
         <v>2318</v>
       </c>
       <c r="I38" t="n">
-        <v>441.921997857886</v>
+        <v>449.728371586774</v>
       </c>
       <c r="J38" t="s">
         <v>11</v>
@@ -16223,7 +16223,7 @@
         <v>44958</v>
       </c>
       <c r="B39" t="n">
-        <v>2778.42784440527</v>
+        <v>2782.05728511067</v>
       </c>
       <c r="C39" t="n">
         <v>21.1720384087052</v>
@@ -16244,7 +16244,7 @@
         <v>5662</v>
       </c>
       <c r="I39" t="n">
-        <v>-2883.57215559473</v>
+        <v>-2879.94271488933</v>
       </c>
       <c r="J39" t="s">
         <v>12</v>
@@ -16255,7 +16255,7 @@
         <v>44986</v>
       </c>
       <c r="B40" t="n">
-        <v>4530.92531528916</v>
+        <v>4523.17101329208</v>
       </c>
       <c r="C40" t="n">
         <v>1669.54752072239</v>
@@ -16276,7 +16276,7 @@
         <v>6543</v>
       </c>
       <c r="I40" t="n">
-        <v>-2012.07468471084</v>
+        <v>-2019.82898670792</v>
       </c>
       <c r="J40" t="s">
         <v>12</v>
@@ -16287,7 +16287,7 @@
         <v>45017</v>
       </c>
       <c r="B41" t="n">
-        <v>5122.77697327965</v>
+        <v>5123.81189797239</v>
       </c>
       <c r="C41" t="n">
         <v>1932.26686118833</v>
@@ -16308,7 +16308,7 @@
         <v>7677</v>
       </c>
       <c r="I41" t="n">
-        <v>-2554.22302672035</v>
+        <v>-2553.18810202761</v>
       </c>
       <c r="J41" t="s">
         <v>12</v>
@@ -16319,7 +16319,7 @@
         <v>45047</v>
       </c>
       <c r="B42" t="n">
-        <v>5866.10913885715</v>
+        <v>5856.75102862987</v>
       </c>
       <c r="C42" t="n">
         <v>2627.20828193442</v>
@@ -16340,7 +16340,7 @@
         <v>9067</v>
       </c>
       <c r="I42" t="n">
-        <v>-3200.89086114285</v>
+        <v>-3210.24897137013</v>
       </c>
       <c r="J42" t="s">
         <v>12</v>
@@ -16351,7 +16351,7 @@
         <v>45078</v>
       </c>
       <c r="B43" t="n">
-        <v>6103.49759345003</v>
+        <v>6092.18601367048</v>
       </c>
       <c r="C43" t="n">
         <v>2728.52603772469</v>
@@ -16372,7 +16372,7 @@
         <v>8326</v>
       </c>
       <c r="I43" t="n">
-        <v>-2222.50240654997</v>
+        <v>-2233.81398632952</v>
       </c>
       <c r="J43" t="s">
         <v>12</v>
@@ -16383,7 +16383,7 @@
         <v>45108</v>
       </c>
       <c r="B44" t="n">
-        <v>6043.32368687703</v>
+        <v>6034.19512033109</v>
       </c>
       <c r="C44" t="n">
         <v>2678.26442334632</v>
@@ -16404,7 +16404,7 @@
         <v>9164</v>
       </c>
       <c r="I44" t="n">
-        <v>-3120.67631312297</v>
+        <v>-3129.80487966891</v>
       </c>
       <c r="J44" t="s">
         <v>12</v>
@@ -16415,7 +16415,7 @@
         <v>45139</v>
       </c>
       <c r="B45" t="n">
-        <v>5389.69270239897</v>
+        <v>5382.84815066267</v>
       </c>
       <c r="C45" t="n">
         <v>1789.30200171136</v>
@@ -16436,7 +16436,7 @@
         <v>8354</v>
       </c>
       <c r="I45" t="n">
-        <v>-2964.30729760103</v>
+        <v>-2971.15184933733</v>
       </c>
       <c r="J45" t="s">
         <v>12</v>
@@ -16447,7 +16447,7 @@
         <v>45170</v>
       </c>
       <c r="B46" t="n">
-        <v>4275.81194968036</v>
+        <v>4263.70931807919</v>
       </c>
       <c r="C46" t="n">
         <v>395.375252653696</v>
@@ -16468,7 +16468,7 @@
         <v>5987</v>
       </c>
       <c r="I46" t="n">
-        <v>-1711.18805031964</v>
+        <v>-1723.29068192081</v>
       </c>
       <c r="J46" t="s">
         <v>12</v>
@@ -16479,7 +16479,7 @@
         <v>45200</v>
       </c>
       <c r="B47" t="n">
-        <v>3346.11887515032</v>
+        <v>3349.13548913693</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -16500,7 +16500,7 @@
         <v>4477</v>
       </c>
       <c r="I47" t="n">
-        <v>-1130.88112484968</v>
+        <v>-1127.86451086307</v>
       </c>
       <c r="J47" t="s">
         <v>12</v>
@@ -16511,7 +16511,7 @@
         <v>45231</v>
       </c>
       <c r="B48" t="n">
-        <v>3273.86880762687</v>
+        <v>3298.1434527773</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -16532,7 +16532,7 @@
         <v>4540</v>
       </c>
       <c r="I48" t="n">
-        <v>-1266.13119237313</v>
+        <v>-1241.8565472227</v>
       </c>
       <c r="J48" t="s">
         <v>12</v>
@@ -16543,7 +16543,7 @@
         <v>45261</v>
       </c>
       <c r="B49" t="n">
-        <v>3275.07690706682</v>
+        <v>3290.41384559314</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -16564,7 +16564,7 @@
         <v>3743</v>
       </c>
       <c r="I49" t="n">
-        <v>-467.923092933183</v>
+        <v>-452.58615440686</v>
       </c>
       <c r="J49" t="s">
         <v>12</v>
@@ -19401,7 +19401,7 @@
         <v>43831</v>
       </c>
       <c r="B2" t="n">
-        <v>817.942145736892</v>
+        <v>847.075291566498</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -19422,7 +19422,7 @@
         <v>71</v>
       </c>
       <c r="I2" t="n">
-        <v>746.942145736892</v>
+        <v>776.075291566498</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
@@ -19433,7 +19433,7 @@
         <v>43862</v>
       </c>
       <c r="B3" t="n">
-        <v>860.670408729624</v>
+        <v>913.113600822468</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -19442,10 +19442,10 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>8386.0428641169</v>
+        <v>14513.4058476909</v>
       </c>
       <c r="F3" t="n">
-        <v>10977.5293603918</v>
+        <v>19161.3945939318</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
@@ -19454,7 +19454,7 @@
         <v>17</v>
       </c>
       <c r="I3" t="n">
-        <v>843.670408729624</v>
+        <v>896.113600822468</v>
       </c>
       <c r="J3" t="s">
         <v>11</v>
@@ -19465,7 +19465,7 @@
         <v>43891</v>
       </c>
       <c r="B4" t="n">
-        <v>849.359048292623</v>
+        <v>873.343687398966</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -19474,10 +19474,10 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>25513.2648999557</v>
+        <v>26401.577264679</v>
       </c>
       <c r="F4" t="n">
-        <v>26908.2500649081</v>
+        <v>27599.6457141782</v>
       </c>
       <c r="G4" t="s">
         <v>31</v>
@@ -19486,7 +19486,7 @@
         <v>16</v>
       </c>
       <c r="I4" t="n">
-        <v>833.359048292623</v>
+        <v>857.343687398966</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
@@ -19497,7 +19497,7 @@
         <v>43922</v>
       </c>
       <c r="B5" t="n">
-        <v>843.848037384715</v>
+        <v>804.368036961116</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -19506,10 +19506,10 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>27351.5775271252</v>
+        <v>28470.7165698227</v>
       </c>
       <c r="F5" t="n">
-        <v>28486.2124924389</v>
+        <v>30785.0787579297</v>
       </c>
       <c r="G5" t="s">
         <v>31</v>
@@ -19518,7 +19518,7 @@
         <v>6</v>
       </c>
       <c r="I5" t="n">
-        <v>837.848037384715</v>
+        <v>798.368036961116</v>
       </c>
       <c r="J5" t="s">
         <v>11</v>
@@ -19529,7 +19529,7 @@
         <v>43952</v>
       </c>
       <c r="B6" t="n">
-        <v>862.728007911249</v>
+        <v>768.158517901678</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -19538,10 +19538,10 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>27350.9843615233</v>
+        <v>25817.0056005935</v>
       </c>
       <c r="F6" t="n">
-        <v>29156.4756064634</v>
+        <v>30448.9070976511</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -19550,7 +19550,7 @@
         <v>4</v>
       </c>
       <c r="I6" t="n">
-        <v>858.728007911249</v>
+        <v>764.158517901678</v>
       </c>
       <c r="J6" t="s">
         <v>11</v>
@@ -19561,7 +19561,7 @@
         <v>43983</v>
       </c>
       <c r="B7" t="n">
-        <v>966.960345046587</v>
+        <v>872.896989631306</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -19570,10 +19570,10 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>25839.678497908</v>
+        <v>22385.3310348867</v>
       </c>
       <c r="F7" t="n">
-        <v>28990.5192554174</v>
+        <v>28189.9995906823</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
@@ -19582,7 +19582,7 @@
         <v>4</v>
       </c>
       <c r="I7" t="n">
-        <v>962.960345046587</v>
+        <v>868.896989631306</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
@@ -19593,7 +19593,7 @@
         <v>44013</v>
       </c>
       <c r="B8" t="n">
-        <v>1661.17118826683</v>
+        <v>2801.44181433936</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -19602,10 +19602,10 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>23718.9165026055</v>
+        <v>20255.2268980556</v>
       </c>
       <c r="F8" t="n">
-        <v>27094.6982794367</v>
+        <v>28374.4394431433</v>
       </c>
       <c r="G8" t="s">
         <v>31</v>
@@ -19614,7 +19614,7 @@
         <v>55</v>
       </c>
       <c r="I8" t="n">
-        <v>1606.17118826683</v>
+        <v>2746.44181433936</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
@@ -19625,7 +19625,7 @@
         <v>44044</v>
       </c>
       <c r="B9" t="n">
-        <v>5699.32275799102</v>
+        <v>7491.71855079946</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -19634,10 +19634,10 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>25291.3220739735</v>
+        <v>27136.9027609581</v>
       </c>
       <c r="F9" t="n">
-        <v>28144.7891359056</v>
+        <v>29472.2004348286</v>
       </c>
       <c r="G9" t="s">
         <v>31</v>
@@ -19646,7 +19646,7 @@
         <v>55</v>
       </c>
       <c r="I9" t="n">
-        <v>5644.32275799102</v>
+        <v>7436.71855079946</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
@@ -19657,7 +19657,7 @@
         <v>44075</v>
       </c>
       <c r="B10" t="n">
-        <v>8458.03959980724</v>
+        <v>9404.14348768957</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -19666,10 +19666,10 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>27190.4088858839</v>
+        <v>28821.876482196</v>
       </c>
       <c r="F10" t="n">
-        <v>28537.6067241244</v>
+        <v>30253.8200463862</v>
       </c>
       <c r="G10" t="s">
         <v>31</v>
@@ -19678,7 +19678,7 @@
         <v>247</v>
       </c>
       <c r="I10" t="n">
-        <v>8211.03959980724</v>
+        <v>9157.14348768957</v>
       </c>
       <c r="J10" t="s">
         <v>11</v>
@@ -19689,7 +19689,7 @@
         <v>44105</v>
       </c>
       <c r="B11" t="n">
-        <v>2353.31275021888</v>
+        <v>2591.93046816105</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -19698,10 +19698,10 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>28760.1630072013</v>
+        <v>26270.697049455</v>
       </c>
       <c r="F11" t="n">
-        <v>30506.0224755143</v>
+        <v>29757.58235898</v>
       </c>
       <c r="G11" t="s">
         <v>31</v>
@@ -19710,7 +19710,7 @@
         <v>287</v>
       </c>
       <c r="I11" t="n">
-        <v>2066.31275021888</v>
+        <v>2304.93046816105</v>
       </c>
       <c r="J11" t="s">
         <v>11</v>
@@ -19721,7 +19721,7 @@
         <v>44136</v>
       </c>
       <c r="B12" t="n">
-        <v>748.418476765822</v>
+        <v>767.057694474272</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -19730,10 +19730,10 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>26448.7299638065</v>
+        <v>25780.4898323606</v>
       </c>
       <c r="F12" t="n">
-        <v>29221.6844930635</v>
+        <v>31551.6628322063</v>
       </c>
       <c r="G12" t="s">
         <v>31</v>
@@ -19742,7 +19742,7 @@
         <v>63</v>
       </c>
       <c r="I12" t="n">
-        <v>685.418476765822</v>
+        <v>704.057694474272</v>
       </c>
       <c r="J12" t="s">
         <v>11</v>
@@ -19753,7 +19753,7 @@
         <v>44166</v>
       </c>
       <c r="B13" t="n">
-        <v>2359.76341907902</v>
+        <v>535.672843741601</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -19762,10 +19762,10 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>24717.6806801242</v>
+        <v>24171.247471249</v>
       </c>
       <c r="F13" t="n">
-        <v>26525.9675782682</v>
+        <v>27685.3278601056</v>
       </c>
       <c r="G13" t="s">
         <v>31</v>
@@ -19774,7 +19774,7 @@
         <v>9</v>
       </c>
       <c r="I13" t="n">
-        <v>2350.76341907902</v>
+        <v>526.672843741601</v>
       </c>
       <c r="J13" t="s">
         <v>11</v>
@@ -19785,7 +19785,7 @@
         <v>44197</v>
       </c>
       <c r="B14" t="n">
-        <v>6789.31259520084</v>
+        <v>4365.58240912582</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -19794,10 +19794,10 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>25286.5452346114</v>
+        <v>25897.9714762342</v>
       </c>
       <c r="F14" t="n">
-        <v>26808.963606062</v>
+        <v>30842.352333515</v>
       </c>
       <c r="G14" t="s">
         <v>31</v>
@@ -19806,7 +19806,7 @@
         <v>5</v>
       </c>
       <c r="I14" t="n">
-        <v>6784.31259520084</v>
+        <v>4360.58240912582</v>
       </c>
       <c r="J14" t="s">
         <v>11</v>
@@ -19817,7 +19817,7 @@
         <v>44228</v>
       </c>
       <c r="B15" t="n">
-        <v>7734.10899759924</v>
+        <v>6649.45576702342</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -19826,10 +19826,10 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>27917.8180984696</v>
+        <v>26020.6368805509</v>
       </c>
       <c r="F15" t="n">
-        <v>29893.2946629904</v>
+        <v>29477.8385117311</v>
       </c>
       <c r="G15" t="s">
         <v>31</v>
@@ -19838,7 +19838,7 @@
         <v>2</v>
       </c>
       <c r="I15" t="n">
-        <v>7732.10899759924</v>
+        <v>6647.45576702342</v>
       </c>
       <c r="J15" t="s">
         <v>11</v>
@@ -19849,7 +19849,7 @@
         <v>44256</v>
       </c>
       <c r="B16" t="n">
-        <v>1148.53978385253</v>
+        <v>1423.87363090197</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -19858,10 +19858,10 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>28498.4863641265</v>
+        <v>26687.9705043815</v>
       </c>
       <c r="F16" t="n">
-        <v>30819.8970134641</v>
+        <v>30376.4199761066</v>
       </c>
       <c r="G16" t="s">
         <v>31</v>
@@ -19870,7 +19870,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>1148.53978385253</v>
+        <v>1423.87363090197</v>
       </c>
       <c r="J16" t="s">
         <v>11</v>
@@ -19881,7 +19881,7 @@
         <v>44287</v>
       </c>
       <c r="B17" t="n">
-        <v>835.676733375404</v>
+        <v>943.351465622423</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -19890,10 +19890,10 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>26858.6216333894</v>
+        <v>24702.979546397</v>
       </c>
       <c r="F17" t="n">
-        <v>29310.7315662531</v>
+        <v>29762.0712390468</v>
       </c>
       <c r="G17" t="s">
         <v>31</v>
@@ -19902,7 +19902,7 @@
         <v>4</v>
       </c>
       <c r="I17" t="n">
-        <v>831.676733375404</v>
+        <v>939.351465622423</v>
       </c>
       <c r="J17" t="s">
         <v>11</v>
@@ -19913,7 +19913,7 @@
         <v>44317</v>
       </c>
       <c r="B18" t="n">
-        <v>2509.40261775401</v>
+        <v>718.42914235533</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -19922,10 +19922,10 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>25835.5882868606</v>
+        <v>25430.0917514203</v>
       </c>
       <c r="F18" t="n">
-        <v>28772.1115823634</v>
+        <v>29922.4235328341</v>
       </c>
       <c r="G18" t="s">
         <v>31</v>
@@ -19934,7 +19934,7 @@
         <v>5</v>
       </c>
       <c r="I18" t="n">
-        <v>2504.40261775401</v>
+        <v>713.42914235533</v>
       </c>
       <c r="J18" t="s">
         <v>11</v>
@@ -19945,7 +19945,7 @@
         <v>44348</v>
       </c>
       <c r="B19" t="n">
-        <v>7253.50464198855</v>
+        <v>781.3152704005</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -19954,10 +19954,10 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>26019.9759634807</v>
+        <v>25180.7344960282</v>
       </c>
       <c r="F19" t="n">
-        <v>28174.2165527149</v>
+        <v>29343.6285646175</v>
       </c>
       <c r="G19" t="s">
         <v>31</v>
@@ -19966,7 +19966,7 @@
         <v>8</v>
       </c>
       <c r="I19" t="n">
-        <v>7245.50464198855</v>
+        <v>773.3152704005</v>
       </c>
       <c r="J19" t="s">
         <v>11</v>
@@ -19977,7 +19977,7 @@
         <v>44378</v>
       </c>
       <c r="B20" t="n">
-        <v>8568.01616338875</v>
+        <v>2699.21538642316</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -19986,10 +19986,10 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>27413.5133042071</v>
+        <v>26257.9966818849</v>
       </c>
       <c r="F20" t="n">
-        <v>29814.7648308991</v>
+        <v>30083.4652522355</v>
       </c>
       <c r="G20" t="s">
         <v>31</v>
@@ -19998,7 +19998,7 @@
         <v>3</v>
       </c>
       <c r="I20" t="n">
-        <v>8565.01616338875</v>
+        <v>2696.21538642316</v>
       </c>
       <c r="J20" t="s">
         <v>11</v>
@@ -20009,7 +20009,7 @@
         <v>44409</v>
       </c>
       <c r="B21" t="n">
-        <v>1268.58642770444</v>
+        <v>8531.07580120204</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -20018,10 +20018,10 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>27680.7290317536</v>
+        <v>25661.5366437233</v>
       </c>
       <c r="F21" t="n">
-        <v>29739.2514511745</v>
+        <v>30109.0007396044</v>
       </c>
       <c r="G21" t="s">
         <v>31</v>
@@ -20030,7 +20030,7 @@
         <v>3</v>
       </c>
       <c r="I21" t="n">
-        <v>1265.58642770444</v>
+        <v>8528.07580120204</v>
       </c>
       <c r="J21" t="s">
         <v>11</v>
@@ -20041,7 +20041,7 @@
         <v>44440</v>
       </c>
       <c r="B22" t="n">
-        <v>1566.54816429478</v>
+        <v>9405.56444144889</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -20050,10 +20050,10 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>26793.8979811473</v>
+        <v>24804.5553362376</v>
       </c>
       <c r="F22" t="n">
-        <v>30591.3385716606</v>
+        <v>29928.7391221569</v>
       </c>
       <c r="G22" t="s">
         <v>31</v>
@@ -20062,7 +20062,7 @@
         <v>4</v>
       </c>
       <c r="I22" t="n">
-        <v>1562.54816429478</v>
+        <v>9401.56444144889</v>
       </c>
       <c r="J22" t="s">
         <v>11</v>
@@ -20073,7 +20073,7 @@
         <v>44470</v>
       </c>
       <c r="B23" t="n">
-        <v>3687.32545442112</v>
+        <v>2539.72336276682</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -20082,10 +20082,10 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>25847.7666184127</v>
+        <v>24609.6417805165</v>
       </c>
       <c r="F23" t="n">
-        <v>29277.8772617967</v>
+        <v>29277.6443746191</v>
       </c>
       <c r="G23" t="s">
         <v>31</v>
@@ -20094,7 +20094,7 @@
         <v>6</v>
       </c>
       <c r="I23" t="n">
-        <v>3681.32545442112</v>
+        <v>2533.72336276682</v>
       </c>
       <c r="J23" t="s">
         <v>11</v>
@@ -20105,7 +20105,7 @@
         <v>44501</v>
       </c>
       <c r="B24" t="n">
-        <v>6399.57497597284</v>
+        <v>1077.0379066697</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -20114,10 +20114,10 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>25330.9786885301</v>
+        <v>25293.0547257383</v>
       </c>
       <c r="F24" t="n">
-        <v>28262.2822575894</v>
+        <v>29425.6441928015</v>
       </c>
       <c r="G24" t="s">
         <v>31</v>
@@ -20126,7 +20126,7 @@
         <v>5</v>
       </c>
       <c r="I24" t="n">
-        <v>6394.57497597284</v>
+        <v>1072.0379066697</v>
       </c>
       <c r="J24" t="s">
         <v>11</v>
@@ -20137,7 +20137,7 @@
         <v>44531</v>
       </c>
       <c r="B25" t="n">
-        <v>7848.46003734564</v>
+        <v>3933.71187954029</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -20146,10 +20146,10 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>26941.5911641336</v>
+        <v>25587.3756709538</v>
       </c>
       <c r="F25" t="n">
-        <v>28866.5145890803</v>
+        <v>29747.2250291626</v>
       </c>
       <c r="G25" t="s">
         <v>31</v>
@@ -20158,7 +20158,7 @@
         <v>3</v>
       </c>
       <c r="I25" t="n">
-        <v>7845.46003734564</v>
+        <v>3930.71187954029</v>
       </c>
       <c r="J25" t="s">
         <v>11</v>
@@ -20169,7 +20169,7 @@
         <v>44562</v>
       </c>
       <c r="B26" t="n">
-        <v>1069.97111331375</v>
+        <v>7868.60398471358</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
@@ -20178,10 +20178,10 @@
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>27936.137022234</v>
+        <v>25588.3392147415</v>
       </c>
       <c r="F26" t="n">
-        <v>30141.1634335818</v>
+        <v>29434.6378270221</v>
       </c>
       <c r="G26" t="s">
         <v>31</v>
@@ -20190,7 +20190,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>1069.97111331375</v>
+        <v>7868.60398471358</v>
       </c>
       <c r="J26" t="s">
         <v>11</v>
@@ -20201,7 +20201,7 @@
         <v>44593</v>
       </c>
       <c r="B27" t="n">
-        <v>673.320512712977</v>
+        <v>2289.08889670286</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -20210,10 +20210,10 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>27314.8759781171</v>
+        <v>24945.1300952832</v>
       </c>
       <c r="F27" t="n">
-        <v>29348.8778263072</v>
+        <v>29331.2938714023</v>
       </c>
       <c r="G27" t="s">
         <v>31</v>
@@ -20222,7 +20222,7 @@
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>673.320512712977</v>
+        <v>2289.08889670286</v>
       </c>
       <c r="J27" t="s">
         <v>11</v>
@@ -20233,7 +20233,7 @@
         <v>44621</v>
       </c>
       <c r="B28" t="n">
-        <v>2507.8065680696</v>
+        <v>989.688073776308</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -20242,10 +20242,10 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>26671.5713616757</v>
+        <v>24534.0665065867</v>
       </c>
       <c r="F28" t="n">
-        <v>29125.216439608</v>
+        <v>29193.0590513298</v>
       </c>
       <c r="G28" t="s">
         <v>31</v>
@@ -20254,7 +20254,7 @@
         <v>2</v>
       </c>
       <c r="I28" t="n">
-        <v>2505.8065680696</v>
+        <v>987.688073776308</v>
       </c>
       <c r="J28" t="s">
         <v>11</v>
@@ -20265,7 +20265,7 @@
         <v>44652</v>
       </c>
       <c r="B29" t="n">
-        <v>6723.86536610251</v>
+        <v>943.165888389078</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -20274,10 +20274,10 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>25652.7814486684</v>
+        <v>24467.4471720606</v>
       </c>
       <c r="F29" t="n">
-        <v>28803.5832545506</v>
+        <v>28105.725864882</v>
       </c>
       <c r="G29" t="s">
         <v>31</v>
@@ -20286,7 +20286,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>6723.86536610251</v>
+        <v>943.165888389078</v>
       </c>
       <c r="J29" t="s">
         <v>11</v>
@@ -20297,7 +20297,7 @@
         <v>44682</v>
       </c>
       <c r="B30" t="n">
-        <v>7883.41562774932</v>
+        <v>928.671761649338</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -20306,10 +20306,10 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>27319.0532210982</v>
+        <v>25092.7539750966</v>
       </c>
       <c r="F30" t="n">
-        <v>29030.2747739211</v>
+        <v>29202.2959619171</v>
       </c>
       <c r="G30" t="s">
         <v>31</v>
@@ -20318,7 +20318,7 @@
         <v>2</v>
       </c>
       <c r="I30" t="n">
-        <v>7881.41562774932</v>
+        <v>926.671761649338</v>
       </c>
       <c r="J30" t="s">
         <v>11</v>
@@ -20329,7 +20329,7 @@
         <v>44713</v>
       </c>
       <c r="B31" t="n">
-        <v>1074.2101755812</v>
+        <v>840.297476512401</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -20338,10 +20338,10 @@
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>27796.1387837937</v>
+        <v>25109.3099550197</v>
       </c>
       <c r="F31" t="n">
-        <v>29848.6287861395</v>
+        <v>29510.2188365378</v>
       </c>
       <c r="G31" t="s">
         <v>31</v>
@@ -20350,7 +20350,7 @@
         <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>1073.2101755812</v>
+        <v>839.297476512401</v>
       </c>
       <c r="J31" t="s">
         <v>11</v>
@@ -20361,7 +20361,7 @@
         <v>44743</v>
       </c>
       <c r="B32" t="n">
-        <v>720.804249650832</v>
+        <v>893.831089053108</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -20370,10 +20370,10 @@
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>27146.1772730664</v>
+        <v>24923.594318524</v>
       </c>
       <c r="F32" t="n">
-        <v>29173.8121696593</v>
+        <v>29318.3205080882</v>
       </c>
       <c r="G32" t="s">
         <v>31</v>
@@ -20382,7 +20382,7 @@
         <v>3</v>
       </c>
       <c r="I32" t="n">
-        <v>717.804249650832</v>
+        <v>890.831089053108</v>
       </c>
       <c r="J32" t="s">
         <v>11</v>
@@ -20393,7 +20393,7 @@
         <v>44774</v>
       </c>
       <c r="B33" t="n">
-        <v>2706.92916133566</v>
+        <v>1301.82244061276</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -20402,10 +20402,10 @@
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>26490.5697775581</v>
+        <v>24203.1944124103</v>
       </c>
       <c r="F33" t="n">
-        <v>29090.4460326349</v>
+        <v>29427.9826162046</v>
       </c>
       <c r="G33" t="s">
         <v>31</v>
@@ -20414,7 +20414,7 @@
         <v>1</v>
       </c>
       <c r="I33" t="n">
-        <v>2705.92916133566</v>
+        <v>1300.82244061276</v>
       </c>
       <c r="J33" t="s">
         <v>11</v>
@@ -20425,7 +20425,7 @@
         <v>44805</v>
       </c>
       <c r="B34" t="n">
-        <v>7330.62275774991</v>
+        <v>2058.33662052074</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -20434,10 +20434,10 @@
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>26042.3562523126</v>
+        <v>24741.8132591975</v>
       </c>
       <c r="F34" t="n">
-        <v>29038.5811745567</v>
+        <v>29307.8800528495</v>
       </c>
       <c r="G34" t="s">
         <v>31</v>
@@ -20446,7 +20446,7 @@
         <v>28</v>
       </c>
       <c r="I34" t="n">
-        <v>7302.62275774991</v>
+        <v>2030.33662052074</v>
       </c>
       <c r="J34" t="s">
         <v>11</v>
@@ -20457,7 +20457,7 @@
         <v>44835</v>
       </c>
       <c r="B35" t="n">
-        <v>9072.031262771</v>
+        <v>2326.67549831816</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -20466,10 +20466,10 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>27387.330820839</v>
+        <v>24642.2408479387</v>
       </c>
       <c r="F35" t="n">
-        <v>30088.7838000293</v>
+        <v>28025.1887817003</v>
       </c>
       <c r="G35" t="s">
         <v>31</v>
@@ -20478,7 +20478,7 @@
         <v>326</v>
       </c>
       <c r="I35" t="n">
-        <v>8746.031262771</v>
+        <v>2000.67549831816</v>
       </c>
       <c r="J35" t="s">
         <v>11</v>
@@ -20489,7 +20489,7 @@
         <v>44866</v>
       </c>
       <c r="B36" t="n">
-        <v>1231.015531428</v>
+        <v>1154.62487137429</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -20498,10 +20498,10 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>27702.02433481</v>
+        <v>24886.7603865702</v>
       </c>
       <c r="F36" t="n">
-        <v>30114.4842989086</v>
+        <v>28911.4927533708</v>
       </c>
       <c r="G36" t="s">
         <v>31</v>
@@ -20510,7 +20510,7 @@
         <v>174</v>
       </c>
       <c r="I36" t="n">
-        <v>1057.015531428</v>
+        <v>980.624871374293</v>
       </c>
       <c r="J36" t="s">
         <v>11</v>
@@ -20521,7 +20521,7 @@
         <v>44896</v>
       </c>
       <c r="B37" t="n">
-        <v>627.6366382347</v>
+        <v>643.547902309514</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -20530,10 +20530,10 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>27196.3975926689</v>
+        <v>24588.7282504884</v>
       </c>
       <c r="F37" t="n">
-        <v>29139.1308491206</v>
+        <v>29317.5157455403</v>
       </c>
       <c r="G37" t="s">
         <v>31</v>
@@ -20542,7 +20542,7 @@
         <v>11</v>
       </c>
       <c r="I37" t="n">
-        <v>616.6366382347</v>
+        <v>632.547902309514</v>
       </c>
       <c r="J37" t="s">
         <v>11</v>
@@ -20553,7 +20553,7 @@
         <v>44927</v>
       </c>
       <c r="B38" t="n">
-        <v>2508.20775852307</v>
+        <v>670.384209072374</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -20562,10 +20562,10 @@
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>26660.1981349244</v>
+        <v>24533.7892821377</v>
       </c>
       <c r="F38" t="n">
-        <v>29231.8184176067</v>
+        <v>28857.9096069961</v>
       </c>
       <c r="G38" t="s">
         <v>31</v>
@@ -20574,7 +20574,7 @@
         <v>1</v>
       </c>
       <c r="I38" t="n">
-        <v>2507.20775852307</v>
+        <v>669.384209072374</v>
       </c>
       <c r="J38" t="s">
         <v>11</v>
@@ -20585,7 +20585,7 @@
         <v>44958</v>
       </c>
       <c r="B39" t="n">
-        <v>6437.12481757583</v>
+        <v>2439.18315279665</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -20594,10 +20594,10 @@
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>26123.8880309284</v>
+        <v>24685.7345448222</v>
       </c>
       <c r="F39" t="n">
-        <v>28636.0126325875</v>
+        <v>28323.3144748625</v>
       </c>
       <c r="G39" t="s">
         <v>31</v>
@@ -20606,7 +20606,7 @@
         <v>11</v>
       </c>
       <c r="I39" t="n">
-        <v>6426.12481757583</v>
+        <v>2428.18315279665</v>
       </c>
       <c r="J39" t="s">
         <v>11</v>
@@ -20617,7 +20617,7 @@
         <v>44986</v>
       </c>
       <c r="B40" t="n">
-        <v>7886.4552581561</v>
+        <v>6648.76327740294</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -20626,10 +20626,10 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>27114.9258670391</v>
+        <v>25109.3353830864</v>
       </c>
       <c r="F40" t="n">
-        <v>29410.8143180527</v>
+        <v>29330.7072155352</v>
       </c>
       <c r="G40" t="s">
         <v>31</v>
@@ -20638,7 +20638,7 @@
         <v>7</v>
       </c>
       <c r="I40" t="n">
-        <v>7879.4552581561</v>
+        <v>6641.76327740294</v>
       </c>
       <c r="J40" t="s">
         <v>11</v>
@@ -20649,7 +20649,7 @@
         <v>45017</v>
       </c>
       <c r="B41" t="n">
-        <v>1051.66931992096</v>
+        <v>8372.88607673883</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -20658,10 +20658,10 @@
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>27663.6184444851</v>
+        <v>25017.7242472758</v>
       </c>
       <c r="F41" t="n">
-        <v>30161.0868529462</v>
+        <v>29546.0433652543</v>
       </c>
       <c r="G41" t="s">
         <v>31</v>
@@ -20670,7 +20670,7 @@
         <v>9</v>
       </c>
       <c r="I41" t="n">
-        <v>1042.66931992096</v>
+        <v>8363.88607673883</v>
       </c>
       <c r="J41" t="s">
         <v>11</v>
@@ -20681,7 +20681,7 @@
         <v>45047</v>
       </c>
       <c r="B42" t="n">
-        <v>669.323881457603</v>
+        <v>1421.1656865157</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -20690,10 +20690,10 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>27717.2735540276</v>
+        <v>24594.8169040304</v>
       </c>
       <c r="F42" t="n">
-        <v>29913.6616237004</v>
+        <v>28629.0448971896</v>
       </c>
       <c r="G42" t="s">
         <v>31</v>
@@ -20702,7 +20702,7 @@
         <v>21</v>
       </c>
       <c r="I42" t="n">
-        <v>648.323881457603</v>
+        <v>1400.1656865157</v>
       </c>
       <c r="J42" t="s">
         <v>11</v>
@@ -20713,7 +20713,7 @@
         <v>45078</v>
       </c>
       <c r="B43" t="n">
-        <v>2512.44417635221</v>
+        <v>938.3109931658</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -20722,10 +20722,10 @@
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>27077.5165393674</v>
+        <v>24246.6876735933</v>
       </c>
       <c r="F43" t="n">
-        <v>29175.8644323549</v>
+        <v>28976.7527383391</v>
       </c>
       <c r="G43" t="s">
         <v>31</v>
@@ -20734,7 +20734,7 @@
         <v>55</v>
       </c>
       <c r="I43" t="n">
-        <v>2457.44417635221</v>
+        <v>883.3109931658</v>
       </c>
       <c r="J43" t="s">
         <v>11</v>
@@ -20745,7 +20745,7 @@
         <v>45108</v>
       </c>
       <c r="B44" t="n">
-        <v>6484.60507144326</v>
+        <v>2594.93497206554</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -20754,10 +20754,10 @@
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>26636.1325350145</v>
+        <v>24537.2933156225</v>
       </c>
       <c r="F44" t="n">
-        <v>28987.4625787071</v>
+        <v>28900.461024956</v>
       </c>
       <c r="G44" t="s">
         <v>31</v>
@@ -20766,7 +20766,7 @@
         <v>1604</v>
       </c>
       <c r="I44" t="n">
-        <v>4880.60507144326</v>
+        <v>990.934972065544</v>
       </c>
       <c r="J44" t="s">
         <v>11</v>
@@ -20777,7 +20777,7 @@
         <v>45139</v>
       </c>
       <c r="B45" t="n">
-        <v>8101.6190590376</v>
+        <v>7738.79860852168</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -20786,10 +20786,10 @@
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>27076.6595635934</v>
+        <v>24829.7007011125</v>
       </c>
       <c r="F45" t="n">
-        <v>29350.7181045267</v>
+        <v>29153.4726335583</v>
       </c>
       <c r="G45" t="s">
         <v>31</v>
@@ -20798,7 +20798,7 @@
         <v>4198</v>
       </c>
       <c r="I45" t="n">
-        <v>3903.6190590376</v>
+        <v>3540.79860852168</v>
       </c>
       <c r="J45" t="s">
         <v>11</v>
@@ -20809,7 +20809,7 @@
         <v>45170</v>
       </c>
       <c r="B46" t="n">
-        <v>1953.94530590777</v>
+        <v>9953.52449308995</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -20818,10 +20818,10 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>27690.6871155319</v>
+        <v>24835.8724402211</v>
       </c>
       <c r="F46" t="n">
-        <v>29924.1997442081</v>
+        <v>29398.1708991756</v>
       </c>
       <c r="G46" t="s">
         <v>31</v>
@@ -20830,10 +20830,10 @@
         <v>6494</v>
       </c>
       <c r="I46" t="n">
-        <v>-4540.05469409223</v>
+        <v>3459.52449308995</v>
       </c>
       <c r="J46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47">
@@ -20841,7 +20841,7 @@
         <v>45200</v>
       </c>
       <c r="B47" t="n">
-        <v>1851.31083476664</v>
+        <v>2594.70073627843</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -20850,10 +20850,10 @@
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>27233.3681663152</v>
+        <v>24232.4896612571</v>
       </c>
       <c r="F47" t="n">
-        <v>29739.6654318192</v>
+        <v>28452.720926765</v>
       </c>
       <c r="G47" t="s">
         <v>31</v>
@@ -20862,7 +20862,7 @@
         <v>5388</v>
       </c>
       <c r="I47" t="n">
-        <v>-3536.68916523336</v>
+        <v>-2793.29926372157</v>
       </c>
       <c r="J47" t="s">
         <v>12</v>
@@ -20873,7 +20873,7 @@
         <v>45231</v>
       </c>
       <c r="B48" t="n">
-        <v>2669.25682892677</v>
+        <v>1074.34416803354</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -20882,10 +20882,10 @@
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>27038.357717323</v>
+        <v>24368.6256054778</v>
       </c>
       <c r="F48" t="n">
-        <v>29258.3799142418</v>
+        <v>28701.3595740803</v>
       </c>
       <c r="G48" t="s">
         <v>31</v>
@@ -20894,10 +20894,10 @@
         <v>1685</v>
       </c>
       <c r="I48" t="n">
-        <v>984.256828926773</v>
+        <v>-610.655831966462</v>
       </c>
       <c r="J48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49">
@@ -20905,7 +20905,7 @@
         <v>45261</v>
       </c>
       <c r="B49" t="n">
-        <v>6391.45373193083</v>
+        <v>3830.93016461334</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -20914,10 +20914,10 @@
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>26700.0360809351</v>
+        <v>24951.6954901552</v>
       </c>
       <c r="F49" t="n">
-        <v>28855.9825907052</v>
+        <v>29407.2011896377</v>
       </c>
       <c r="G49" t="s">
         <v>31</v>
@@ -20926,7 +20926,7 @@
         <v>154</v>
       </c>
       <c r="I49" t="n">
-        <v>6237.45373193083</v>
+        <v>3676.93016461334</v>
       </c>
       <c r="J49" t="s">
         <v>11</v>
@@ -25682,10 +25682,10 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>272.279923767045</v>
+        <v>254.978138622258</v>
       </c>
       <c r="F3" t="n">
-        <v>376.139268956894</v>
+        <v>359.692968632402</v>
       </c>
       <c r="G3" t="s">
         <v>35</v>
@@ -25714,10 +25714,10 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>338.419389486532</v>
+        <v>301.607225189755</v>
       </c>
       <c r="F4" t="n">
-        <v>594.582242952781</v>
+        <v>448.894554900978</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
@@ -25746,10 +25746,10 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>809.177138029519</v>
+        <v>601.324735147575</v>
       </c>
       <c r="F5" t="n">
-        <v>1773.29082615962</v>
+        <v>1247.45976570351</v>
       </c>
       <c r="G5" t="s">
         <v>35</v>
@@ -25778,10 +25778,10 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>958.228866907608</v>
+        <v>768.928802655745</v>
       </c>
       <c r="F6" t="n">
-        <v>1836.71051527942</v>
+        <v>1438.17264810886</v>
       </c>
       <c r="G6" t="s">
         <v>35</v>
@@ -25801,7 +25801,7 @@
         <v>43983</v>
       </c>
       <c r="B7" t="n">
-        <v>4.35266208834269</v>
+        <v>2.27381621367978</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -25810,10 +25810,10 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>708.332797798918</v>
+        <v>544.578837438132</v>
       </c>
       <c r="F7" t="n">
-        <v>1688.32782491095</v>
+        <v>1203.66923960347</v>
       </c>
       <c r="G7" t="s">
         <v>35</v>
@@ -25822,7 +25822,7 @@
         <v>6</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.64733791165731</v>
+        <v>-3.72618378632022</v>
       </c>
       <c r="J7" t="s">
         <v>12</v>
@@ -25833,7 +25833,7 @@
         <v>44013</v>
       </c>
       <c r="B8" t="n">
-        <v>134.332626104082</v>
+        <v>128.666225377227</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -25842,10 +25842,10 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>910.688753799615</v>
+        <v>654.396529078582</v>
       </c>
       <c r="F8" t="n">
-        <v>1932.11887577842</v>
+        <v>1465.25206642596</v>
       </c>
       <c r="G8" t="s">
         <v>35</v>
@@ -25854,7 +25854,7 @@
         <v>69</v>
       </c>
       <c r="I8" t="n">
-        <v>65.332626104082</v>
+        <v>59.6662253772271</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
@@ -25865,7 +25865,7 @@
         <v>44044</v>
       </c>
       <c r="B9" t="n">
-        <v>343.357194826915</v>
+        <v>340.465096986078</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -25874,10 +25874,10 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>1180.19602482982</v>
+        <v>939.264048144212</v>
       </c>
       <c r="F9" t="n">
-        <v>2094.14024395584</v>
+        <v>1602.8287961124</v>
       </c>
       <c r="G9" t="s">
         <v>35</v>
@@ -25886,7 +25886,7 @@
         <v>69</v>
       </c>
       <c r="I9" t="n">
-        <v>274.357194826915</v>
+        <v>271.465096986078</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
@@ -25897,7 +25897,7 @@
         <v>44075</v>
       </c>
       <c r="B10" t="n">
-        <v>204.319548580356</v>
+        <v>208.450482066848</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -25906,10 +25906,10 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1054.47438632673</v>
+        <v>796.223578999396</v>
       </c>
       <c r="F10" t="n">
-        <v>1997.9092242857</v>
+        <v>1487.26456139706</v>
       </c>
       <c r="G10" t="s">
         <v>35</v>
@@ -25918,7 +25918,7 @@
         <v>137</v>
       </c>
       <c r="I10" t="n">
-        <v>67.3195485803562</v>
+        <v>71.4504820668477</v>
       </c>
       <c r="J10" t="s">
         <v>11</v>
@@ -25929,7 +25929,7 @@
         <v>44105</v>
       </c>
       <c r="B11" t="n">
-        <v>47.2539700323799</v>
+        <v>54.9824535964919</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -25938,10 +25938,10 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>752.558107320874</v>
+        <v>578.154910677943</v>
       </c>
       <c r="F11" t="n">
-        <v>1806.74993186705</v>
+        <v>1351.33633918474</v>
       </c>
       <c r="G11" t="s">
         <v>35</v>
@@ -25950,7 +25950,7 @@
         <v>42</v>
       </c>
       <c r="I11" t="n">
-        <v>5.25397003237985</v>
+        <v>12.9824535964919</v>
       </c>
       <c r="J11" t="s">
         <v>11</v>
@@ -25970,10 +25970,10 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>529.35192150308</v>
+        <v>520.782994662582</v>
       </c>
       <c r="F12" t="n">
-        <v>1590.79294421306</v>
+        <v>1132.60021207638</v>
       </c>
       <c r="G12" t="s">
         <v>35</v>
@@ -26005,7 +26005,7 @@
         <v>540.275085515153</v>
       </c>
       <c r="F13" t="n">
-        <v>1516.33198772952</v>
+        <v>1043.06483211359</v>
       </c>
       <c r="G13" t="s">
         <v>35</v>
@@ -26034,10 +26034,10 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>750.01497554733</v>
+        <v>554.474684315649</v>
       </c>
       <c r="F14" t="n">
-        <v>1710.16154334685</v>
+        <v>1173.44828744567</v>
       </c>
       <c r="G14" t="s">
         <v>35</v>
@@ -26057,7 +26057,7 @@
         <v>44228</v>
       </c>
       <c r="B15" t="n">
-        <v>15.7977731064104</v>
+        <v>0.0736080827840944</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -26066,10 +26066,10 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>1181.87851704323</v>
+        <v>873.024726509974</v>
       </c>
       <c r="F15" t="n">
-        <v>1931.03679022431</v>
+        <v>1494.91606565094</v>
       </c>
       <c r="G15" t="s">
         <v>35</v>
@@ -26078,7 +26078,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>15.7977731064104</v>
+        <v>0.0736080827840944</v>
       </c>
       <c r="J15" t="s">
         <v>11</v>
@@ -26089,7 +26089,7 @@
         <v>44256</v>
       </c>
       <c r="B16" t="n">
-        <v>16.5384715139995</v>
+        <v>10.7961920147094</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -26098,10 +26098,10 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>1332.82038271736</v>
+        <v>981.321326573523</v>
       </c>
       <c r="F16" t="n">
-        <v>1961.85593652343</v>
+        <v>1532.07993251643</v>
       </c>
       <c r="G16" t="s">
         <v>35</v>
@@ -26110,7 +26110,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>16.5384715139995</v>
+        <v>10.7961920147094</v>
       </c>
       <c r="J16" t="s">
         <v>11</v>
@@ -26130,10 +26130,10 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>1340.98504526097</v>
+        <v>965.346477532478</v>
       </c>
       <c r="F17" t="n">
-        <v>2192.58104204746</v>
+        <v>1610.29335679672</v>
       </c>
       <c r="G17" t="s">
         <v>35</v>
@@ -26162,10 +26162,10 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>1304.93752568308</v>
+        <v>987.826132585542</v>
       </c>
       <c r="F18" t="n">
-        <v>2482.81380371492</v>
+        <v>1983.76800899424</v>
       </c>
       <c r="G18" t="s">
         <v>35</v>
@@ -26194,10 +26194,10 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>1136.66054678825</v>
+        <v>914.170394632834</v>
       </c>
       <c r="F19" t="n">
-        <v>2123.58898430062</v>
+        <v>1694.63913104194</v>
       </c>
       <c r="G19" t="s">
         <v>35</v>
@@ -26217,7 +26217,7 @@
         <v>44378</v>
       </c>
       <c r="B20" t="n">
-        <v>120.215168978794</v>
+        <v>110.723154951442</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -26226,10 +26226,10 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>1167.39135659596</v>
+        <v>851.723696579942</v>
       </c>
       <c r="F20" t="n">
-        <v>2235.25377251154</v>
+        <v>1663.0893061776</v>
       </c>
       <c r="G20" t="s">
         <v>35</v>
@@ -26238,7 +26238,7 @@
         <v>17</v>
       </c>
       <c r="I20" t="n">
-        <v>103.215168978794</v>
+        <v>93.7231549514422</v>
       </c>
       <c r="J20" t="s">
         <v>11</v>
@@ -26249,7 +26249,7 @@
         <v>44409</v>
       </c>
       <c r="B21" t="n">
-        <v>356.119712194118</v>
+        <v>335.476116248648</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -26258,10 +26258,10 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>1635.33754000482</v>
+        <v>1187.55630152838</v>
       </c>
       <c r="F21" t="n">
-        <v>2479.88131981096</v>
+        <v>1842.32015949287</v>
       </c>
       <c r="G21" t="s">
         <v>35</v>
@@ -26270,7 +26270,7 @@
         <v>72</v>
       </c>
       <c r="I21" t="n">
-        <v>284.119712194118</v>
+        <v>263.476116248648</v>
       </c>
       <c r="J21" t="s">
         <v>11</v>
@@ -26281,7 +26281,7 @@
         <v>44440</v>
       </c>
       <c r="B22" t="n">
-        <v>243.050429060495</v>
+        <v>234.510692885332</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -26290,10 +26290,10 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>1600.0083812537</v>
+        <v>1212.64994068625</v>
       </c>
       <c r="F22" t="n">
-        <v>2504.185736382</v>
+        <v>1968.55517119565</v>
       </c>
       <c r="G22" t="s">
         <v>35</v>
@@ -26302,7 +26302,7 @@
         <v>63</v>
       </c>
       <c r="I22" t="n">
-        <v>180.050429060495</v>
+        <v>171.510692885332</v>
       </c>
       <c r="J22" t="s">
         <v>11</v>
@@ -26313,7 +26313,7 @@
         <v>44470</v>
       </c>
       <c r="B23" t="n">
-        <v>75.401347394458</v>
+        <v>83.1130949616459</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -26322,10 +26322,10 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>1611.45079047532</v>
+        <v>1195.46628780686</v>
       </c>
       <c r="F23" t="n">
-        <v>2411.25526239101</v>
+        <v>1921.90537147396</v>
       </c>
       <c r="G23" t="s">
         <v>35</v>
@@ -26334,7 +26334,7 @@
         <v>39</v>
       </c>
       <c r="I23" t="n">
-        <v>36.401347394458</v>
+        <v>44.1130949616459</v>
       </c>
       <c r="J23" t="s">
         <v>11</v>
@@ -26345,7 +26345,7 @@
         <v>44501</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>7.82597877361967</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -26354,10 +26354,10 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>1136.64092569656</v>
+        <v>811.776356939282</v>
       </c>
       <c r="F24" t="n">
-        <v>1981.17024201667</v>
+        <v>1452.05990202354</v>
       </c>
       <c r="G24" t="s">
         <v>35</v>
@@ -26366,7 +26366,7 @@
         <v>14</v>
       </c>
       <c r="I24" t="n">
-        <v>-14</v>
+        <v>-6.17402122638033</v>
       </c>
       <c r="J24" t="s">
         <v>12</v>
@@ -26386,10 +26386,10 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>982.027637490357</v>
+        <v>757.313050655695</v>
       </c>
       <c r="F25" t="n">
-        <v>2052.63198601384</v>
+        <v>1625.06819155231</v>
       </c>
       <c r="G25" t="s">
         <v>35</v>
@@ -26418,10 +26418,10 @@
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>1055.4067162723</v>
+        <v>760.43129878723</v>
       </c>
       <c r="F26" t="n">
-        <v>2191.07727569148</v>
+        <v>1709.77872326811</v>
       </c>
       <c r="G26" t="s">
         <v>35</v>
@@ -26441,7 +26441,7 @@
         <v>44593</v>
       </c>
       <c r="B27" t="n">
-        <v>10.720985649363</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -26450,10 +26450,10 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>1636.91771744021</v>
+        <v>1160.32257148498</v>
       </c>
       <c r="F27" t="n">
-        <v>2376.39788332858</v>
+        <v>1835.02068496425</v>
       </c>
       <c r="G27" t="s">
         <v>35</v>
@@ -26462,10 +26462,10 @@
         <v>1</v>
       </c>
       <c r="I27" t="n">
-        <v>9.72098564936296</v>
+        <v>-1</v>
       </c>
       <c r="J27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28">
@@ -26473,7 +26473,7 @@
         <v>44621</v>
       </c>
       <c r="B28" t="n">
-        <v>68.1688554698061</v>
+        <v>35.5985814042469</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -26482,10 +26482,10 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>1777.00598447955</v>
+        <v>1410.37736156058</v>
       </c>
       <c r="F28" t="n">
-        <v>2462.66599855949</v>
+        <v>1935.46815587777</v>
       </c>
       <c r="G28" t="s">
         <v>35</v>
@@ -26494,7 +26494,7 @@
         <v>2</v>
       </c>
       <c r="I28" t="n">
-        <v>66.1688554698061</v>
+        <v>33.5985814042469</v>
       </c>
       <c r="J28" t="s">
         <v>11</v>
@@ -26505,7 +26505,7 @@
         <v>44652</v>
       </c>
       <c r="B29" t="n">
-        <v>35.7211122581728</v>
+        <v>37.9130259817929</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -26514,10 +26514,10 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>1561.81972320947</v>
+        <v>1120.84299270834</v>
       </c>
       <c r="F29" t="n">
-        <v>2437.27750858359</v>
+        <v>1962.92995275388</v>
       </c>
       <c r="G29" t="s">
         <v>35</v>
@@ -26526,7 +26526,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>35.7211122581728</v>
+        <v>37.9130259817929</v>
       </c>
       <c r="J29" t="s">
         <v>11</v>
@@ -26546,10 +26546,10 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>1595.11801281309</v>
+        <v>1208.16431370196</v>
       </c>
       <c r="F30" t="n">
-        <v>2594.19523974546</v>
+        <v>2036.62938102858</v>
       </c>
       <c r="G30" t="s">
         <v>35</v>
@@ -26578,10 +26578,10 @@
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>1286.27656860569</v>
+        <v>1042.38061536435</v>
       </c>
       <c r="F31" t="n">
-        <v>2452.63300683367</v>
+        <v>2091.3429109561</v>
       </c>
       <c r="G31" t="s">
         <v>35</v>
@@ -26601,7 +26601,7 @@
         <v>44743</v>
       </c>
       <c r="B32" t="n">
-        <v>98.0363820878814</v>
+        <v>92.8317112176975</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -26610,10 +26610,10 @@
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>1397.69834659753</v>
+        <v>1082.73464097861</v>
       </c>
       <c r="F32" t="n">
-        <v>2418.35658929398</v>
+        <v>1862.29010932523</v>
       </c>
       <c r="G32" t="s">
         <v>35</v>
@@ -26622,7 +26622,7 @@
         <v>13</v>
       </c>
       <c r="I32" t="n">
-        <v>85.0363820878814</v>
+        <v>79.8317112176975</v>
       </c>
       <c r="J32" t="s">
         <v>11</v>
@@ -26633,7 +26633,7 @@
         <v>44774</v>
       </c>
       <c r="B33" t="n">
-        <v>324.724383066685</v>
+        <v>310.790561157857</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -26642,10 +26642,10 @@
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>1641.42162989311</v>
+        <v>1366.98797933007</v>
       </c>
       <c r="F33" t="n">
-        <v>2578.61096176462</v>
+        <v>2171.93339014986</v>
       </c>
       <c r="G33" t="s">
         <v>35</v>
@@ -26654,7 +26654,7 @@
         <v>57</v>
       </c>
       <c r="I33" t="n">
-        <v>267.724383066685</v>
+        <v>253.790561157857</v>
       </c>
       <c r="J33" t="s">
         <v>11</v>
@@ -26665,7 +26665,7 @@
         <v>44805</v>
       </c>
       <c r="B34" t="n">
-        <v>272.626380285965</v>
+        <v>244.665092082335</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -26674,10 +26674,10 @@
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>1810.04190625779</v>
+        <v>1422.93610939132</v>
       </c>
       <c r="F34" t="n">
-        <v>2603.66458683305</v>
+        <v>2087.75855554226</v>
       </c>
       <c r="G34" t="s">
         <v>35</v>
@@ -26686,7 +26686,7 @@
         <v>53</v>
       </c>
       <c r="I34" t="n">
-        <v>219.626380285965</v>
+        <v>191.665092082335</v>
       </c>
       <c r="J34" t="s">
         <v>11</v>
@@ -26697,7 +26697,7 @@
         <v>44835</v>
       </c>
       <c r="B35" t="n">
-        <v>123.26553377236</v>
+        <v>130.214616337173</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -26706,10 +26706,10 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>1798.40717869001</v>
+        <v>1352.66907128059</v>
       </c>
       <c r="F35" t="n">
-        <v>2661.61862067523</v>
+        <v>2309.75513314184</v>
       </c>
       <c r="G35" t="s">
         <v>35</v>
@@ -26718,7 +26718,7 @@
         <v>27</v>
       </c>
       <c r="I35" t="n">
-        <v>96.2655337723598</v>
+        <v>103.214616337173</v>
       </c>
       <c r="J35" t="s">
         <v>11</v>
@@ -26729,7 +26729,7 @@
         <v>44866</v>
       </c>
       <c r="B36" t="n">
-        <v>23.8983695093955</v>
+        <v>42.4495800982366</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -26738,10 +26738,10 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>1442.72446132164</v>
+        <v>1045.41603705987</v>
       </c>
       <c r="F36" t="n">
-        <v>2394.86392683916</v>
+        <v>1929.55630275681</v>
       </c>
       <c r="G36" t="s">
         <v>35</v>
@@ -26750,7 +26750,7 @@
         <v>1</v>
       </c>
       <c r="I36" t="n">
-        <v>22.8983695093955</v>
+        <v>41.4495800982366</v>
       </c>
       <c r="J36" t="s">
         <v>11</v>
@@ -26770,10 +26770,10 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>1262.23111338339</v>
+        <v>924.129813685913</v>
       </c>
       <c r="F37" t="n">
-        <v>2474.44434230542</v>
+        <v>1939.87490747641</v>
       </c>
       <c r="G37" t="s">
         <v>35</v>
@@ -26802,10 +26802,10 @@
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>1194.24943969272</v>
+        <v>900.144436576483</v>
       </c>
       <c r="F38" t="n">
-        <v>2415.72532781622</v>
+        <v>1820.43014040812</v>
       </c>
       <c r="G38" t="s">
         <v>35</v>
@@ -26834,10 +26834,10 @@
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>1808.7305366805</v>
+        <v>1386.67804516771</v>
       </c>
       <c r="F39" t="n">
-        <v>2688.73623011468</v>
+        <v>2185.96921927416</v>
       </c>
       <c r="G39" t="s">
         <v>35</v>
@@ -26857,7 +26857,7 @@
         <v>44986</v>
       </c>
       <c r="B40" t="n">
-        <v>48.5126779230205</v>
+        <v>9.45860264206813</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -26866,10 +26866,10 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>1921.86043378616</v>
+        <v>1496.43686123418</v>
       </c>
       <c r="F40" t="n">
-        <v>2738.33010574432</v>
+        <v>2202.05986232484</v>
       </c>
       <c r="G40" t="s">
         <v>35</v>
@@ -26878,7 +26878,7 @@
         <v>3</v>
       </c>
       <c r="I40" t="n">
-        <v>45.5126779230205</v>
+        <v>6.45860264206813</v>
       </c>
       <c r="J40" t="s">
         <v>11</v>
@@ -26889,7 +26889,7 @@
         <v>45017</v>
       </c>
       <c r="B41" t="n">
-        <v>89.4028334647075</v>
+        <v>72.9849152134362</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -26898,10 +26898,10 @@
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>1821.5316427118</v>
+        <v>1486.034179702</v>
       </c>
       <c r="F41" t="n">
-        <v>2638.23769106881</v>
+        <v>2246.66894425637</v>
       </c>
       <c r="G41" t="s">
         <v>35</v>
@@ -26910,7 +26910,7 @@
         <v>1</v>
       </c>
       <c r="I41" t="n">
-        <v>88.4028334647075</v>
+        <v>71.9849152134362</v>
       </c>
       <c r="J41" t="s">
         <v>11</v>
@@ -26921,7 +26921,7 @@
         <v>45047</v>
       </c>
       <c r="B42" t="n">
-        <v>24.8420395533744</v>
+        <v>35.8347305774807</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -26930,10 +26930,10 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>1770.61161617574</v>
+        <v>1293.06371296081</v>
       </c>
       <c r="F42" t="n">
-        <v>2604.57765763745</v>
+        <v>2097.27962185932</v>
       </c>
       <c r="G42" t="s">
         <v>35</v>
@@ -26942,7 +26942,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>24.8420395533744</v>
+        <v>35.8347305774807</v>
       </c>
       <c r="J42" t="s">
         <v>11</v>
@@ -26953,7 +26953,7 @@
         <v>45078</v>
       </c>
       <c r="B43" t="n">
-        <v>0</v>
+        <v>1.05504620735705</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -26962,10 +26962,10 @@
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>1609.52311592368</v>
+        <v>1360.47991576257</v>
       </c>
       <c r="F43" t="n">
-        <v>2621.61596967318</v>
+        <v>2316.48569727922</v>
       </c>
       <c r="G43" t="s">
         <v>35</v>
@@ -26974,7 +26974,7 @@
         <v>3</v>
       </c>
       <c r="I43" t="n">
-        <v>-3</v>
+        <v>-1.94495379264295</v>
       </c>
       <c r="J43" t="s">
         <v>12</v>
@@ -26985,7 +26985,7 @@
         <v>45108</v>
       </c>
       <c r="B44" t="n">
-        <v>89.978172586855</v>
+        <v>90.2476490828214</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -26994,10 +26994,10 @@
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>1474.56887799637</v>
+        <v>1184.80528973202</v>
       </c>
       <c r="F44" t="n">
-        <v>2466.35618546785</v>
+        <v>2011.68402622186</v>
       </c>
       <c r="G44" t="s">
         <v>35</v>
@@ -27006,7 +27006,7 @@
         <v>33</v>
       </c>
       <c r="I44" t="n">
-        <v>56.978172586855</v>
+        <v>57.2476490828214</v>
       </c>
       <c r="J44" t="s">
         <v>11</v>
@@ -27017,7 +27017,7 @@
         <v>45139</v>
       </c>
       <c r="B45" t="n">
-        <v>292.814603883655</v>
+        <v>286.771438411819</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -27026,10 +27026,10 @@
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>1764.58358748455</v>
+        <v>1514.99579073141</v>
       </c>
       <c r="F45" t="n">
-        <v>2600.3780679821</v>
+        <v>2099.55985156725</v>
       </c>
       <c r="G45" t="s">
         <v>35</v>
@@ -27038,7 +27038,7 @@
         <v>80</v>
       </c>
       <c r="I45" t="n">
-        <v>212.814603883655</v>
+        <v>206.771438411819</v>
       </c>
       <c r="J45" t="s">
         <v>11</v>
@@ -27049,7 +27049,7 @@
         <v>45170</v>
       </c>
       <c r="B46" t="n">
-        <v>228.718446935428</v>
+        <v>200.503894375854</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -27058,10 +27058,10 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>1859.59397738926</v>
+        <v>1560.04261073404</v>
       </c>
       <c r="F46" t="n">
-        <v>2612.10813392169</v>
+        <v>2191.24604102313</v>
       </c>
       <c r="G46" t="s">
         <v>35</v>
@@ -27070,7 +27070,7 @@
         <v>62</v>
       </c>
       <c r="I46" t="n">
-        <v>166.718446935428</v>
+        <v>138.503894375854</v>
       </c>
       <c r="J46" t="s">
         <v>11</v>
@@ -27081,7 +27081,7 @@
         <v>45200</v>
       </c>
       <c r="B47" t="n">
-        <v>179.909061802052</v>
+        <v>153.999406877275</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -27090,10 +27090,10 @@
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>1779.1913459346</v>
+        <v>1443.50524495038</v>
       </c>
       <c r="F47" t="n">
-        <v>2656.41629829379</v>
+        <v>2311.75722156458</v>
       </c>
       <c r="G47" t="s">
         <v>35</v>
@@ -27102,7 +27102,7 @@
         <v>32</v>
       </c>
       <c r="I47" t="n">
-        <v>147.909061802052</v>
+        <v>121.999406877275</v>
       </c>
       <c r="J47" t="s">
         <v>11</v>
@@ -27113,7 +27113,7 @@
         <v>45231</v>
       </c>
       <c r="B48" t="n">
-        <v>68.0166170863779</v>
+        <v>78.0042928001795</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -27122,10 +27122,10 @@
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>1641.07134500775</v>
+        <v>1356.38925532798</v>
       </c>
       <c r="F48" t="n">
-        <v>2693.30961806135</v>
+        <v>2292.55225304514</v>
       </c>
       <c r="G48" t="s">
         <v>35</v>
@@ -27134,7 +27134,7 @@
         <v>12</v>
       </c>
       <c r="I48" t="n">
-        <v>56.0166170863779</v>
+        <v>66.0042928001795</v>
       </c>
       <c r="J48" t="s">
         <v>11</v>
@@ -27145,7 +27145,7 @@
         <v>45261</v>
       </c>
       <c r="B49" t="n">
-        <v>1.48848010218895</v>
+        <v>11.5414797704154</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -27154,10 +27154,10 @@
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>1748.15621036448</v>
+        <v>1260.28741822718</v>
       </c>
       <c r="F49" t="n">
-        <v>2630.04666887272</v>
+        <v>2071.95209271933</v>
       </c>
       <c r="G49" t="s">
         <v>35</v>
@@ -27166,10 +27166,10 @@
         <v>4</v>
       </c>
       <c r="I49" t="n">
-        <v>-2.51151989781105</v>
+        <v>7.54147977041536</v>
       </c>
       <c r="J49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -30245,7 +30245,7 @@
         <v>43831</v>
       </c>
       <c r="B2" t="n">
-        <v>2375.86527235627</v>
+        <v>2360.39455573452</v>
       </c>
       <c r="C2" t="n">
         <v>2092.67073250141</v>
@@ -30266,7 +30266,7 @@
         <v>1626</v>
       </c>
       <c r="I2" t="n">
-        <v>749.865272356268</v>
+        <v>734.394555734517</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
@@ -30277,7 +30277,7 @@
         <v>43862</v>
       </c>
       <c r="B3" t="n">
-        <v>2369.96478183978</v>
+        <v>2352.32559555366</v>
       </c>
       <c r="C3" t="n">
         <v>1972.65524679747</v>
@@ -30298,7 +30298,7 @@
         <v>1045</v>
       </c>
       <c r="I3" t="n">
-        <v>1324.96478183978</v>
+        <v>1307.32559555366</v>
       </c>
       <c r="J3" t="s">
         <v>11</v>
@@ -30309,10 +30309,10 @@
         <v>43891</v>
       </c>
       <c r="B4" t="n">
-        <v>3145.83049909941</v>
+        <v>3170.93958214168</v>
       </c>
       <c r="C4" t="n">
-        <v>2714.99216292644</v>
+        <v>2821.15113400456</v>
       </c>
       <c r="D4" t="n">
         <v>2617.69890368062</v>
@@ -30330,7 +30330,7 @@
         <v>1641</v>
       </c>
       <c r="I4" t="n">
-        <v>1504.83049909941</v>
+        <v>1529.93958214168</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
@@ -30341,7 +30341,7 @@
         <v>43922</v>
       </c>
       <c r="B5" t="n">
-        <v>2942.79401417899</v>
+        <v>2938.06367494595</v>
       </c>
       <c r="C5" t="n">
         <v>2480.75761103751</v>
@@ -30350,7 +30350,7 @@
         <v>2262.09225504128</v>
       </c>
       <c r="E5" t="n">
-        <v>3327.575655822</v>
+        <v>3307.93184266879</v>
       </c>
       <c r="F5" t="n">
         <v>3526.81419987515</v>
@@ -30362,7 +30362,7 @@
         <v>1732</v>
       </c>
       <c r="I5" t="n">
-        <v>1210.79401417899</v>
+        <v>1206.06367494595</v>
       </c>
       <c r="J5" t="s">
         <v>11</v>
@@ -30373,7 +30373,7 @@
         <v>43952</v>
       </c>
       <c r="B6" t="n">
-        <v>2651.6272239533</v>
+        <v>2614.75849661334</v>
       </c>
       <c r="C6" t="n">
         <v>2089.6139643587</v>
@@ -30382,10 +30382,10 @@
         <v>1924.55013593521</v>
       </c>
       <c r="E6" t="n">
-        <v>3156.23486436951</v>
+        <v>3002.2587283695</v>
       </c>
       <c r="F6" t="n">
-        <v>3188.65956344707</v>
+        <v>3181.78860470656</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
@@ -30394,7 +30394,7 @@
         <v>1585</v>
       </c>
       <c r="I6" t="n">
-        <v>1066.6272239533</v>
+        <v>1029.75849661334</v>
       </c>
       <c r="J6" t="s">
         <v>11</v>
@@ -30405,7 +30405,7 @@
         <v>43983</v>
       </c>
       <c r="B7" t="n">
-        <v>2302.72221694863</v>
+        <v>2238.50348973571</v>
       </c>
       <c r="C7" t="n">
         <v>1761.55378011194</v>
@@ -30414,7 +30414,7 @@
         <v>1589.10435823062</v>
       </c>
       <c r="E7" t="n">
-        <v>2729.17216002548</v>
+        <v>2625.72882298163</v>
       </c>
       <c r="F7" t="n">
         <v>2827.53569070833</v>
@@ -30426,7 +30426,7 @@
         <v>1708</v>
       </c>
       <c r="I7" t="n">
-        <v>594.722216948628</v>
+        <v>530.503489735707</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
@@ -30437,7 +30437,7 @@
         <v>44013</v>
       </c>
       <c r="B8" t="n">
-        <v>2284.71699478346</v>
+        <v>2250.84188571033</v>
       </c>
       <c r="C8" t="n">
         <v>1784.29864013751</v>
@@ -30458,7 +30458,7 @@
         <v>1759</v>
       </c>
       <c r="I8" t="n">
-        <v>525.716994783462</v>
+        <v>491.841885710326</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
@@ -30469,7 +30469,7 @@
         <v>44044</v>
       </c>
       <c r="B9" t="n">
-        <v>2209.63653161118</v>
+        <v>2251.51253617101</v>
       </c>
       <c r="C9" t="n">
         <v>1789.86011713188</v>
@@ -30490,7 +30490,7 @@
         <v>1759</v>
       </c>
       <c r="I9" t="n">
-        <v>450.636531611178</v>
+        <v>492.51253617101</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
@@ -30501,7 +30501,7 @@
         <v>44075</v>
       </c>
       <c r="B10" t="n">
-        <v>2013.88686497512</v>
+        <v>2024.69787883702</v>
       </c>
       <c r="C10" t="n">
         <v>1531.74947334365</v>
@@ -30522,7 +30522,7 @@
         <v>1811</v>
       </c>
       <c r="I10" t="n">
-        <v>202.886864975116</v>
+        <v>213.69787883702</v>
       </c>
       <c r="J10" t="s">
         <v>11</v>
@@ -30533,7 +30533,7 @@
         <v>44105</v>
       </c>
       <c r="B11" t="n">
-        <v>1860.00167916912</v>
+        <v>1853.53740933331</v>
       </c>
       <c r="C11" t="n">
         <v>1364.39386169921</v>
@@ -30554,7 +30554,7 @@
         <v>1506</v>
       </c>
       <c r="I11" t="n">
-        <v>354.001679169116</v>
+        <v>347.537409333307</v>
       </c>
       <c r="J11" t="s">
         <v>11</v>
@@ -30565,7 +30565,7 @@
         <v>44136</v>
       </c>
       <c r="B12" t="n">
-        <v>1989.24031042648</v>
+        <v>2014.47765952703</v>
       </c>
       <c r="C12" t="n">
         <v>1579.53111299129</v>
@@ -30586,7 +30586,7 @@
         <v>1639</v>
       </c>
       <c r="I12" t="n">
-        <v>350.240310426483</v>
+        <v>375.477659527029</v>
       </c>
       <c r="J12" t="s">
         <v>11</v>
@@ -30597,7 +30597,7 @@
         <v>44166</v>
       </c>
       <c r="B13" t="n">
-        <v>2060.53299468797</v>
+        <v>2082.13414466569</v>
       </c>
       <c r="C13" t="n">
         <v>1596.77428920028</v>
@@ -30618,7 +30618,7 @@
         <v>1818</v>
       </c>
       <c r="I13" t="n">
-        <v>242.532994687968</v>
+        <v>264.134144665692</v>
       </c>
       <c r="J13" t="s">
         <v>11</v>
@@ -30629,7 +30629,7 @@
         <v>44197</v>
       </c>
       <c r="B14" t="n">
-        <v>2366.22120019795</v>
+        <v>2379.62098943604</v>
       </c>
       <c r="C14" t="n">
         <v>1914.43103099402</v>
@@ -30650,7 +30650,7 @@
         <v>1838</v>
       </c>
       <c r="I14" t="n">
-        <v>528.221200197948</v>
+        <v>541.620989436036</v>
       </c>
       <c r="J14" t="s">
         <v>11</v>
@@ -30661,7 +30661,7 @@
         <v>44228</v>
       </c>
       <c r="B15" t="n">
-        <v>2359.46631273279</v>
+        <v>2375.27561271413</v>
       </c>
       <c r="C15" t="n">
         <v>1768.52726544701</v>
@@ -30682,7 +30682,7 @@
         <v>1849</v>
       </c>
       <c r="I15" t="n">
-        <v>510.466312732785</v>
+        <v>526.275612714135</v>
       </c>
       <c r="J15" t="s">
         <v>11</v>
@@ -30693,10 +30693,10 @@
         <v>44256</v>
       </c>
       <c r="B16" t="n">
-        <v>3136.10662498193</v>
+        <v>3085.37024305792</v>
       </c>
       <c r="C16" t="n">
-        <v>2631.44449876311</v>
+        <v>2465.74140743452</v>
       </c>
       <c r="D16" t="n">
         <v>2384.98025229264</v>
@@ -30714,7 +30714,7 @@
         <v>2991</v>
       </c>
       <c r="I16" t="n">
-        <v>145.10662498193</v>
+        <v>94.3702430579224</v>
       </c>
       <c r="J16" t="s">
         <v>11</v>
@@ -30725,7 +30725,7 @@
         <v>44287</v>
       </c>
       <c r="B17" t="n">
-        <v>2999.01293911684</v>
+        <v>2922.68121387256</v>
       </c>
       <c r="C17" t="n">
         <v>2329.24592105384</v>
@@ -30734,7 +30734,7 @@
         <v>2030.04324651397</v>
       </c>
       <c r="E17" t="n">
-        <v>3598.65790962952</v>
+        <v>3459.66053386259</v>
       </c>
       <c r="F17" t="n">
         <v>3758.86320840246</v>
@@ -30746,7 +30746,7 @@
         <v>2797</v>
       </c>
       <c r="I17" t="n">
-        <v>202.012939116835</v>
+        <v>125.681213872556</v>
       </c>
       <c r="J17" t="s">
         <v>11</v>
@@ -30757,7 +30757,7 @@
         <v>44317</v>
       </c>
       <c r="B18" t="n">
-        <v>2676.72473795193</v>
+        <v>2654.48048423851</v>
       </c>
       <c r="C18" t="n">
         <v>1949.79547507638</v>
@@ -30766,7 +30766,7 @@
         <v>1710.71620936223</v>
       </c>
       <c r="E18" t="n">
-        <v>3309.19840176694</v>
+        <v>3196.43259445353</v>
       </c>
       <c r="F18" t="n">
         <v>3411.45727795734</v>
@@ -30778,7 +30778,7 @@
         <v>2509</v>
       </c>
       <c r="I18" t="n">
-        <v>167.724737951929</v>
+        <v>145.480484238507</v>
       </c>
       <c r="J18" t="s">
         <v>11</v>
@@ -30789,7 +30789,7 @@
         <v>44348</v>
       </c>
       <c r="B19" t="n">
-        <v>2336.10801843763</v>
+        <v>2275.20377989122</v>
       </c>
       <c r="C19" t="n">
         <v>1625.94413108705</v>
@@ -30798,7 +30798,7 @@
         <v>1381.7072973625</v>
       </c>
       <c r="E19" t="n">
-        <v>2897.30942524766</v>
+        <v>2780.7649372921</v>
       </c>
       <c r="F19" t="n">
         <v>3064.64296638977</v>
@@ -30810,7 +30810,7 @@
         <v>2266</v>
       </c>
       <c r="I19" t="n">
-        <v>70.108018437626</v>
+        <v>9.20377989122335</v>
       </c>
       <c r="J19" t="s">
         <v>11</v>
@@ -30821,7 +30821,7 @@
         <v>44378</v>
       </c>
       <c r="B20" t="n">
-        <v>2278.15850798352</v>
+        <v>2225.56607818956</v>
       </c>
       <c r="C20" t="n">
         <v>1652.52589758054</v>
@@ -30842,7 +30842,7 @@
         <v>2140</v>
       </c>
       <c r="I20" t="n">
-        <v>138.158507983517</v>
+        <v>85.5660781895554</v>
       </c>
       <c r="J20" t="s">
         <v>11</v>
@@ -30853,7 +30853,7 @@
         <v>44409</v>
       </c>
       <c r="B21" t="n">
-        <v>2234.13048153406</v>
+        <v>2234.12562072625</v>
       </c>
       <c r="C21" t="n">
         <v>1661.60572536473</v>
@@ -30874,7 +30874,7 @@
         <v>2109</v>
       </c>
       <c r="I21" t="n">
-        <v>125.13048153406</v>
+        <v>125.125620726247</v>
       </c>
       <c r="J21" t="s">
         <v>11</v>
@@ -30885,7 +30885,7 @@
         <v>44440</v>
       </c>
       <c r="B22" t="n">
-        <v>2047.45234301031</v>
+        <v>2040.98833102556</v>
       </c>
       <c r="C22" t="n">
         <v>1386.06673025111</v>
@@ -30906,7 +30906,7 @@
         <v>2033</v>
       </c>
       <c r="I22" t="n">
-        <v>14.4523430103106</v>
+        <v>7.98833102555818</v>
       </c>
       <c r="J22" t="s">
         <v>11</v>
@@ -30917,7 +30917,7 @@
         <v>44470</v>
       </c>
       <c r="B23" t="n">
-        <v>1862.45774225095</v>
+        <v>1892.94888338909</v>
       </c>
       <c r="C23" t="n">
         <v>1213.91124407118</v>
@@ -30938,7 +30938,7 @@
         <v>1846</v>
       </c>
       <c r="I23" t="n">
-        <v>16.4577422509494</v>
+        <v>46.9488833890862</v>
       </c>
       <c r="J23" t="s">
         <v>11</v>
@@ -30949,7 +30949,7 @@
         <v>44501</v>
       </c>
       <c r="B24" t="n">
-        <v>1973.05346778722</v>
+        <v>2007.09868395807</v>
       </c>
       <c r="C24" t="n">
         <v>1434.67903069169</v>
@@ -30970,7 +30970,7 @@
         <v>2055</v>
       </c>
       <c r="I24" t="n">
-        <v>-81.9465322127794</v>
+        <v>-47.9013160419336</v>
       </c>
       <c r="J24" t="s">
         <v>12</v>
@@ -30981,7 +30981,7 @@
         <v>44531</v>
       </c>
       <c r="B25" t="n">
-        <v>2056.44163062415</v>
+        <v>2081.45596042113</v>
       </c>
       <c r="C25" t="n">
         <v>1456.22526462817</v>
@@ -31002,7 +31002,7 @@
         <v>2369</v>
       </c>
       <c r="I25" t="n">
-        <v>-312.558369375852</v>
+        <v>-287.544039578875</v>
       </c>
       <c r="J25" t="s">
         <v>12</v>
@@ -31013,7 +31013,7 @@
         <v>44562</v>
       </c>
       <c r="B26" t="n">
-        <v>2349.90331203171</v>
+        <v>2374.73095176211</v>
       </c>
       <c r="C26" t="n">
         <v>1782.8628673287</v>
@@ -31034,7 +31034,7 @@
         <v>2530</v>
       </c>
       <c r="I26" t="n">
-        <v>-180.096687968295</v>
+        <v>-155.269048237889</v>
       </c>
       <c r="J26" t="s">
         <v>12</v>
@@ -31045,7 +31045,7 @@
         <v>44593</v>
       </c>
       <c r="B27" t="n">
-        <v>2356.72074074303</v>
+        <v>2325.42763219352</v>
       </c>
       <c r="C27" t="n">
         <v>1623.85930325603</v>
@@ -31066,7 +31066,7 @@
         <v>2443</v>
       </c>
       <c r="I27" t="n">
-        <v>-86.2792592569749</v>
+        <v>-117.572367806476</v>
       </c>
       <c r="J27" t="s">
         <v>12</v>
@@ -31077,10 +31077,10 @@
         <v>44621</v>
       </c>
       <c r="B28" t="n">
-        <v>3128.13368198304</v>
+        <v>3087.36353973135</v>
       </c>
       <c r="C28" t="n">
-        <v>2574.20138899116</v>
+        <v>2448.47204028956</v>
       </c>
       <c r="D28" t="n">
         <v>2198.76620775587</v>
@@ -31098,7 +31098,7 @@
         <v>3131</v>
       </c>
       <c r="I28" t="n">
-        <v>-2.8663180169624</v>
+        <v>-43.6364602686485</v>
       </c>
       <c r="J28" t="s">
         <v>12</v>
@@ -31109,7 +31109,7 @@
         <v>44652</v>
       </c>
       <c r="B29" t="n">
-        <v>3001.45131297182</v>
+        <v>2834.58864534412</v>
       </c>
       <c r="C29" t="n">
         <v>2164.45414392355</v>
@@ -31118,7 +31118,7 @@
         <v>1826.72430239158</v>
       </c>
       <c r="E29" t="n">
-        <v>3642.01061913805</v>
+        <v>3580.16001318352</v>
       </c>
       <c r="F29" t="n">
         <v>3943.15125889888</v>
@@ -31130,7 +31130,7 @@
         <v>2525</v>
       </c>
       <c r="I29" t="n">
-        <v>476.451312971822</v>
+        <v>309.588645344117</v>
       </c>
       <c r="J29" t="s">
         <v>11</v>
@@ -31141,7 +31141,7 @@
         <v>44682</v>
       </c>
       <c r="B30" t="n">
-        <v>2684.37856019641</v>
+        <v>2637.18996904426</v>
       </c>
       <c r="C30" t="n">
         <v>1843.83249649127</v>
@@ -31150,7 +31150,7 @@
         <v>1499.87471884951</v>
       </c>
       <c r="E30" t="n">
-        <v>3365.87278005652</v>
+        <v>3240.08338226704</v>
       </c>
       <c r="F30" t="n">
         <v>3593.10969167383</v>
@@ -31162,7 +31162,7 @@
         <v>2503</v>
       </c>
       <c r="I30" t="n">
-        <v>181.378560196408</v>
+        <v>134.189969044259</v>
       </c>
       <c r="J30" t="s">
         <v>11</v>
@@ -31173,7 +31173,7 @@
         <v>44713</v>
       </c>
       <c r="B31" t="n">
-        <v>2354.10623332186</v>
+        <v>2303.37397941122</v>
       </c>
       <c r="C31" t="n">
         <v>1521.97792708445</v>
@@ -31182,7 +31182,7 @@
         <v>1183.90265702296</v>
       </c>
       <c r="E31" t="n">
-        <v>2992.1623385381</v>
+        <v>2901.81894926931</v>
       </c>
       <c r="F31" t="n">
         <v>3249.77910139857</v>
@@ -31194,7 +31194,7 @@
         <v>2411</v>
       </c>
       <c r="I31" t="n">
-        <v>-56.8937666781444</v>
+        <v>-107.626020588782</v>
       </c>
       <c r="J31" t="s">
         <v>12</v>
@@ -31205,7 +31205,7 @@
         <v>44743</v>
       </c>
       <c r="B32" t="n">
-        <v>2283.9336143542</v>
+        <v>2243.79823076496</v>
       </c>
       <c r="C32" t="n">
         <v>1550.28782413263</v>
@@ -31226,7 +31226,7 @@
         <v>2225</v>
       </c>
       <c r="I32" t="n">
-        <v>58.933614354195</v>
+        <v>18.7982307649622</v>
       </c>
       <c r="J32" t="s">
         <v>11</v>
@@ -31237,7 +31237,7 @@
         <v>44774</v>
       </c>
       <c r="B33" t="n">
-        <v>2219.62630733114</v>
+        <v>2237.96058241431</v>
       </c>
       <c r="C33" t="n">
         <v>1549.03743878369</v>
@@ -31258,7 +31258,7 @@
         <v>2255</v>
       </c>
       <c r="I33" t="n">
-        <v>-35.3736926688593</v>
+        <v>-17.0394175856936</v>
       </c>
       <c r="J33" t="s">
         <v>12</v>
@@ -31269,7 +31269,7 @@
         <v>44805</v>
       </c>
       <c r="B34" t="n">
-        <v>2042.41189525506</v>
+        <v>2057.2892337754</v>
       </c>
       <c r="C34" t="n">
         <v>1270.61212162443</v>
@@ -31290,7 +31290,7 @@
         <v>1946</v>
       </c>
       <c r="I34" t="n">
-        <v>96.4118952550625</v>
+        <v>111.289233775401</v>
       </c>
       <c r="J34" t="s">
         <v>11</v>
@@ -31301,7 +31301,7 @@
         <v>44835</v>
       </c>
       <c r="B35" t="n">
-        <v>1861.78505851484</v>
+        <v>1898.93375166217</v>
       </c>
       <c r="C35" t="n">
         <v>1095.57269499521</v>
@@ -31322,7 +31322,7 @@
         <v>1683</v>
       </c>
       <c r="I35" t="n">
-        <v>178.785058514835</v>
+        <v>215.933751662174</v>
       </c>
       <c r="J35" t="s">
         <v>11</v>
@@ -31333,7 +31333,7 @@
         <v>44866</v>
       </c>
       <c r="B36" t="n">
-        <v>1963.91917901127</v>
+        <v>2016.55427857588</v>
       </c>
       <c r="C36" t="n">
         <v>1318.81651411255</v>
@@ -31354,7 +31354,7 @@
         <v>1732</v>
       </c>
       <c r="I36" t="n">
-        <v>231.919179011272</v>
+        <v>284.554278575883</v>
       </c>
       <c r="J36" t="s">
         <v>11</v>
@@ -31365,7 +31365,7 @@
         <v>44896</v>
       </c>
       <c r="B37" t="n">
-        <v>2059.1246281667</v>
+        <v>2057.19702818581</v>
       </c>
       <c r="C37" t="n">
         <v>1338.80662894613</v>
@@ -31386,7 +31386,7 @@
         <v>1187</v>
       </c>
       <c r="I37" t="n">
-        <v>872.124628166698</v>
+        <v>870.197028185814</v>
       </c>
       <c r="J37" t="s">
         <v>11</v>
@@ -31397,7 +31397,7 @@
         <v>44927</v>
       </c>
       <c r="B38" t="n">
-        <v>2338.39429427472</v>
+        <v>2338.58315343903</v>
       </c>
       <c r="C38" t="n">
         <v>1645.34393971249</v>
@@ -31418,7 +31418,7 @@
         <v>1144</v>
       </c>
       <c r="I38" t="n">
-        <v>1194.39429427472</v>
+        <v>1194.58315343903</v>
       </c>
       <c r="J38" t="s">
         <v>11</v>
@@ -31429,7 +31429,7 @@
         <v>44958</v>
       </c>
       <c r="B39" t="n">
-        <v>2348.53812807094</v>
+        <v>2333.21289648938</v>
       </c>
       <c r="C39" t="n">
         <v>1486.11401111166</v>
@@ -31450,7 +31450,7 @@
         <v>2207</v>
       </c>
       <c r="I39" t="n">
-        <v>141.53812807094</v>
+        <v>126.212896489378</v>
       </c>
       <c r="J39" t="s">
         <v>11</v>
@@ -31461,7 +31461,7 @@
         <v>44986</v>
       </c>
       <c r="B40" t="n">
-        <v>3135.57079399774</v>
+        <v>3083.30892494582</v>
       </c>
       <c r="C40" t="n">
         <v>2405.26410121057</v>
@@ -31482,10 +31482,10 @@
         <v>3117</v>
       </c>
       <c r="I40" t="n">
-        <v>18.5707939977378</v>
+        <v>-33.691075054182</v>
       </c>
       <c r="J40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41">
@@ -31493,7 +31493,7 @@
         <v>45017</v>
       </c>
       <c r="B41" t="n">
-        <v>2993.98946928103</v>
+        <v>2720.44158009397</v>
       </c>
       <c r="C41" t="n">
         <v>1971.63522254429</v>
@@ -31514,7 +31514,7 @@
         <v>3006</v>
       </c>
       <c r="I41" t="n">
-        <v>-12.0105307189656</v>
+        <v>-285.558419906026</v>
       </c>
       <c r="J41" t="s">
         <v>12</v>
@@ -31525,7 +31525,7 @@
         <v>45047</v>
       </c>
       <c r="B42" t="n">
-        <v>2665.33598253778</v>
+        <v>2657.5648211793</v>
       </c>
       <c r="C42" t="n">
         <v>1649.24414445909</v>
@@ -31534,7 +31534,7 @@
         <v>1212.63032751826</v>
       </c>
       <c r="E42" t="n">
-        <v>3388.09142131129</v>
+        <v>3342.17526555114</v>
       </c>
       <c r="F42" t="n">
         <v>3749.24575340589</v>
@@ -31546,7 +31546,7 @@
         <v>2822</v>
       </c>
       <c r="I42" t="n">
-        <v>-156.664017462219</v>
+        <v>-164.435178820697</v>
       </c>
       <c r="J42" t="s">
         <v>12</v>
@@ -31557,7 +31557,7 @@
         <v>45078</v>
       </c>
       <c r="B43" t="n">
-        <v>2353.76568844257</v>
+        <v>2359.02527019689</v>
       </c>
       <c r="C43" t="n">
         <v>1337.62907551692</v>
@@ -31566,7 +31566,7 @@
         <v>893.966327251034</v>
       </c>
       <c r="E43" t="n">
-        <v>3095.57993302711</v>
+        <v>3013.82683868839</v>
       </c>
       <c r="F43" t="n">
         <v>3457.48958695427</v>
@@ -31578,7 +31578,7 @@
         <v>2529</v>
       </c>
       <c r="I43" t="n">
-        <v>-175.234311557428</v>
+        <v>-169.974729803109</v>
       </c>
       <c r="J43" t="s">
         <v>12</v>
@@ -31589,7 +31589,7 @@
         <v>45108</v>
       </c>
       <c r="B44" t="n">
-        <v>2283.34762077196</v>
+        <v>2245.03757081197</v>
       </c>
       <c r="C44" t="n">
         <v>1368.94888135808</v>
@@ -31610,7 +31610,7 @@
         <v>2620</v>
       </c>
       <c r="I44" t="n">
-        <v>-336.652379228036</v>
+        <v>-374.962429188034</v>
       </c>
       <c r="J44" t="s">
         <v>12</v>
@@ -31621,7 +31621,7 @@
         <v>45139</v>
       </c>
       <c r="B45" t="n">
-        <v>2224.30115073114</v>
+        <v>2220.69897041823</v>
       </c>
       <c r="C45" t="n">
         <v>1367.68751238602</v>
@@ -31642,7 +31642,7 @@
         <v>2618</v>
       </c>
       <c r="I45" t="n">
-        <v>-393.69884926886</v>
+        <v>-397.301029581767</v>
       </c>
       <c r="J45" t="s">
         <v>12</v>
@@ -31653,7 +31653,7 @@
         <v>45170</v>
       </c>
       <c r="B46" t="n">
-        <v>2039.23222153562</v>
+        <v>2061.05175497573</v>
       </c>
       <c r="C46" t="n">
         <v>1081.92151510189</v>
@@ -31674,7 +31674,7 @@
         <v>2550</v>
       </c>
       <c r="I46" t="n">
-        <v>-510.767778464377</v>
+        <v>-488.948245024274</v>
       </c>
       <c r="J46" t="s">
         <v>12</v>
@@ -31685,7 +31685,7 @@
         <v>45200</v>
       </c>
       <c r="B47" t="n">
-        <v>1857.21027274206</v>
+        <v>1911.22120405076</v>
       </c>
       <c r="C47" t="n">
         <v>896.641655395377</v>
@@ -31706,7 +31706,7 @@
         <v>2543</v>
       </c>
       <c r="I47" t="n">
-        <v>-685.789727257937</v>
+        <v>-631.778795949243</v>
       </c>
       <c r="J47" t="s">
         <v>12</v>
@@ -31717,7 +31717,7 @@
         <v>45231</v>
       </c>
       <c r="B48" t="n">
-        <v>1957.97043576441</v>
+        <v>2059.46726197347</v>
       </c>
       <c r="C48" t="n">
         <v>1121.84715679139</v>
@@ -31738,7 +31738,7 @@
         <v>2751</v>
       </c>
       <c r="I48" t="n">
-        <v>-793.029564235586</v>
+        <v>-691.532738026527</v>
       </c>
       <c r="J48" t="s">
         <v>12</v>
@@ -31749,7 +31749,7 @@
         <v>45261</v>
       </c>
       <c r="B49" t="n">
-        <v>2047.08304074506</v>
+        <v>2055.77357235953</v>
       </c>
       <c r="C49" t="n">
         <v>1132.11414754105</v>
@@ -31770,7 +31770,7 @@
         <v>2668</v>
       </c>
       <c r="I49" t="n">
-        <v>-620.916959254943</v>
+        <v>-612.226427640468</v>
       </c>
       <c r="J49" t="s">
         <v>12</v>

</xml_diff>